<commit_message>
Modif excel ordo opti III.2
</commit_message>
<xml_diff>
--- a/ordo.xlsx
+++ b/ordo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="34">
   <si>
     <t>P1</t>
   </si>
@@ -141,7 +141,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,12 +151,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -437,7 +431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -457,29 +451,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -800,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CX74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CY9" sqref="CY9:DD17"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AL37" sqref="AL37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -843,17 +836,17 @@
       </c>
     </row>
     <row r="3" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I3" s="42"/>
+      <c r="I3" s="41"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="40"/>
+      <c r="K3" s="39"/>
       <c r="L3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="40"/>
+      <c r="M3" s="39"/>
       <c r="N3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="40"/>
+      <c r="O3" s="39"/>
       <c r="P3" s="2" t="s">
         <v>24</v>
       </c>
@@ -880,18 +873,18 @@
       <c r="G4" s="10">
         <v>6</v>
       </c>
-      <c r="I4" s="43"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="45" t="s">
+      <c r="I4" s="42"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="44"/>
-      <c r="N4" s="45" t="s">
+      <c r="M4" s="43"/>
+      <c r="N4" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="O4" s="44"/>
-      <c r="P4" s="45"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="44"/>
       <c r="AP4" s="1"/>
     </row>
     <row r="5" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -916,7 +909,7 @@
       <c r="G5" s="12">
         <v>20</v>
       </c>
-      <c r="I5" s="43" t="s">
+      <c r="I5" s="42" t="s">
         <v>1</v>
       </c>
       <c r="J5" s="3" t="s">
@@ -964,17 +957,17 @@
       <c r="G6" s="16">
         <v>22</v>
       </c>
-      <c r="I6" s="42"/>
+      <c r="I6" s="41"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="40"/>
+      <c r="K6" s="39"/>
       <c r="L6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="40"/>
+      <c r="M6" s="39"/>
       <c r="N6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O6" s="40"/>
+      <c r="O6" s="39"/>
       <c r="P6" s="2" t="s">
         <v>25</v>
       </c>
@@ -1002,18 +995,18 @@
       <c r="G7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="43"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="44"/>
-      <c r="L7" s="45" t="s">
+      <c r="I7" s="42"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="M7" s="44"/>
-      <c r="N7" s="45" t="s">
+      <c r="M7" s="43"/>
+      <c r="N7" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="O7" s="44"/>
-      <c r="P7" s="45"/>
+      <c r="O7" s="43"/>
+      <c r="P7" s="44"/>
       <c r="AP7" s="1"/>
     </row>
     <row r="8" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1024,572 +1017,572 @@
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="40"/>
-      <c r="L8" s="40"/>
-      <c r="M8" s="40"/>
-      <c r="N8" s="40"/>
-      <c r="O8" s="40"/>
-      <c r="P8" s="40"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="39"/>
+      <c r="P8" s="39"/>
       <c r="AP8" s="1"/>
     </row>
-    <row r="9" spans="1:102" s="35" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="33" t="s">
+    <row r="9" spans="1:102" s="34" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="41">
+      <c r="B9" s="40">
         <v>0</v>
       </c>
-      <c r="C9" s="34">
+      <c r="C9" s="33">
         <v>1</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="33">
         <v>2</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="33">
         <v>3</v>
       </c>
-      <c r="F9" s="34">
+      <c r="F9" s="33">
         <v>4</v>
       </c>
-      <c r="G9" s="34">
+      <c r="G9" s="33">
         <v>5</v>
       </c>
-      <c r="H9" s="34">
+      <c r="H9" s="33">
         <v>6</v>
       </c>
-      <c r="I9" s="34">
+      <c r="I9" s="33">
         <v>7</v>
       </c>
-      <c r="J9" s="34">
+      <c r="J9" s="33">
         <v>8</v>
       </c>
-      <c r="K9" s="34">
+      <c r="K9" s="33">
         <v>9</v>
       </c>
-      <c r="L9" s="34">
+      <c r="L9" s="33">
         <v>10</v>
       </c>
-      <c r="M9" s="34">
-        <v>11</v>
-      </c>
-      <c r="N9" s="34">
+      <c r="M9" s="33">
+        <v>11</v>
+      </c>
+      <c r="N9" s="33">
         <v>12</v>
       </c>
-      <c r="O9" s="34">
+      <c r="O9" s="33">
         <v>13</v>
       </c>
-      <c r="P9" s="34">
+      <c r="P9" s="33">
         <v>14</v>
       </c>
-      <c r="Q9" s="34">
-        <v>15</v>
-      </c>
-      <c r="R9" s="34">
+      <c r="Q9" s="33">
+        <v>15</v>
+      </c>
+      <c r="R9" s="33">
         <v>16</v>
       </c>
-      <c r="S9" s="34">
+      <c r="S9" s="33">
         <v>17</v>
       </c>
-      <c r="T9" s="34">
+      <c r="T9" s="33">
         <v>18</v>
       </c>
-      <c r="U9" s="34">
+      <c r="U9" s="33">
         <v>19</v>
       </c>
-      <c r="V9" s="34">
-        <v>20</v>
-      </c>
-      <c r="W9" s="34">
+      <c r="V9" s="33">
+        <v>20</v>
+      </c>
+      <c r="W9" s="33">
         <v>21</v>
       </c>
-      <c r="X9" s="34">
-        <v>22</v>
-      </c>
-      <c r="Y9" s="34">
-        <v>23</v>
-      </c>
-      <c r="Z9" s="34">
+      <c r="X9" s="33">
+        <v>22</v>
+      </c>
+      <c r="Y9" s="33">
+        <v>23</v>
+      </c>
+      <c r="Z9" s="33">
         <v>24</v>
       </c>
-      <c r="AA9" s="34">
+      <c r="AA9" s="33">
         <v>25</v>
       </c>
-      <c r="AB9" s="34">
+      <c r="AB9" s="33">
         <v>26</v>
       </c>
-      <c r="AC9" s="34">
+      <c r="AC9" s="33">
         <v>27</v>
       </c>
-      <c r="AD9" s="34">
+      <c r="AD9" s="33">
         <v>28</v>
       </c>
-      <c r="AE9" s="34">
+      <c r="AE9" s="33">
         <v>29</v>
       </c>
-      <c r="AF9" s="34">
+      <c r="AF9" s="33">
         <v>30</v>
       </c>
-      <c r="AG9" s="34">
+      <c r="AG9" s="33">
         <v>31</v>
       </c>
-      <c r="AH9" s="34">
+      <c r="AH9" s="33">
         <v>32</v>
       </c>
-      <c r="AI9" s="34">
+      <c r="AI9" s="33">
         <v>33</v>
       </c>
-      <c r="AJ9" s="34">
+      <c r="AJ9" s="33">
         <v>34</v>
       </c>
-      <c r="AK9" s="34">
+      <c r="AK9" s="33">
         <v>35</v>
       </c>
-      <c r="AL9" s="34">
+      <c r="AL9" s="33">
         <v>36</v>
       </c>
-      <c r="AM9" s="34">
+      <c r="AM9" s="33">
         <v>37</v>
       </c>
-      <c r="AN9" s="34">
+      <c r="AN9" s="33">
         <v>38</v>
       </c>
-      <c r="AO9" s="34">
+      <c r="AO9" s="33">
         <v>39</v>
       </c>
-      <c r="AP9" s="34">
+      <c r="AP9" s="33">
         <v>40</v>
       </c>
-      <c r="AQ9" s="34">
+      <c r="AQ9" s="33">
         <v>41</v>
       </c>
-      <c r="AR9" s="34">
+      <c r="AR9" s="33">
         <v>42</v>
       </c>
-      <c r="AS9" s="34">
+      <c r="AS9" s="33">
         <v>43</v>
       </c>
-      <c r="AT9" s="34">
+      <c r="AT9" s="33">
         <v>44</v>
       </c>
-      <c r="AU9" s="34">
+      <c r="AU9" s="33">
         <v>45</v>
       </c>
-      <c r="AV9" s="34">
+      <c r="AV9" s="33">
         <v>46</v>
       </c>
-      <c r="AW9" s="34">
+      <c r="AW9" s="33">
         <v>47</v>
       </c>
-      <c r="AX9" s="34">
+      <c r="AX9" s="33">
         <v>48</v>
       </c>
-      <c r="AY9" s="34">
+      <c r="AY9" s="33">
         <v>49</v>
       </c>
-      <c r="AZ9" s="34">
+      <c r="AZ9" s="33">
         <v>50</v>
       </c>
-      <c r="BA9" s="34">
+      <c r="BA9" s="33">
         <v>51</v>
       </c>
-      <c r="BB9" s="34">
+      <c r="BB9" s="33">
         <v>52</v>
       </c>
-      <c r="BC9" s="34">
+      <c r="BC9" s="33">
         <v>53</v>
       </c>
-      <c r="BD9" s="34">
+      <c r="BD9" s="33">
         <v>54</v>
       </c>
-      <c r="BE9" s="34">
+      <c r="BE9" s="33">
         <v>55</v>
       </c>
-      <c r="BF9" s="34">
+      <c r="BF9" s="33">
         <v>56</v>
       </c>
-      <c r="BG9" s="34">
+      <c r="BG9" s="33">
         <v>57</v>
       </c>
-      <c r="BH9" s="34">
+      <c r="BH9" s="33">
         <v>58</v>
       </c>
-      <c r="BI9" s="34">
+      <c r="BI9" s="33">
         <v>59</v>
       </c>
-      <c r="BJ9" s="34">
+      <c r="BJ9" s="33">
         <v>60</v>
       </c>
-      <c r="BK9" s="34">
+      <c r="BK9" s="33">
         <v>61</v>
       </c>
-      <c r="BL9" s="34">
+      <c r="BL9" s="33">
         <v>62</v>
       </c>
-      <c r="BM9" s="34">
+      <c r="BM9" s="33">
         <v>63</v>
       </c>
-      <c r="BN9" s="34">
+      <c r="BN9" s="33">
         <v>64</v>
       </c>
-      <c r="BO9" s="34">
+      <c r="BO9" s="33">
         <v>65</v>
       </c>
-      <c r="BP9" s="34">
+      <c r="BP9" s="33">
         <v>66</v>
       </c>
-      <c r="BQ9" s="34">
+      <c r="BQ9" s="33">
         <v>67</v>
       </c>
-      <c r="BR9" s="34">
+      <c r="BR9" s="33">
         <v>68</v>
       </c>
-      <c r="BS9" s="34">
+      <c r="BS9" s="33">
         <v>69</v>
       </c>
-      <c r="BT9" s="34">
+      <c r="BT9" s="33">
         <v>70</v>
       </c>
-      <c r="BU9" s="34">
+      <c r="BU9" s="33">
         <v>71</v>
       </c>
-      <c r="BV9" s="34">
+      <c r="BV9" s="33">
         <v>72</v>
       </c>
-      <c r="BW9" s="34">
+      <c r="BW9" s="33">
         <v>73</v>
       </c>
-      <c r="BX9" s="34">
+      <c r="BX9" s="33">
         <v>74</v>
       </c>
-      <c r="BY9" s="34">
+      <c r="BY9" s="33">
         <v>75</v>
       </c>
-      <c r="BZ9" s="34">
+      <c r="BZ9" s="33">
         <v>76</v>
       </c>
-      <c r="CA9" s="34">
+      <c r="CA9" s="33">
         <v>77</v>
       </c>
-      <c r="CB9" s="34">
+      <c r="CB9" s="33">
         <v>78</v>
       </c>
-      <c r="CC9" s="34">
+      <c r="CC9" s="33">
         <v>79</v>
       </c>
-      <c r="CD9" s="34">
+      <c r="CD9" s="33">
         <v>80</v>
       </c>
-      <c r="CE9" s="34">
+      <c r="CE9" s="33">
         <v>81</v>
       </c>
-      <c r="CF9" s="34">
+      <c r="CF9" s="33">
         <v>82</v>
       </c>
-      <c r="CG9" s="34">
+      <c r="CG9" s="33">
         <v>83</v>
       </c>
-      <c r="CH9" s="34">
+      <c r="CH9" s="33">
         <v>84</v>
       </c>
-      <c r="CI9" s="34">
+      <c r="CI9" s="33">
         <v>85</v>
       </c>
-      <c r="CJ9" s="34">
+      <c r="CJ9" s="33">
         <v>86</v>
       </c>
-      <c r="CK9" s="34">
+      <c r="CK9" s="33">
         <v>87</v>
       </c>
-      <c r="CL9" s="34">
+      <c r="CL9" s="33">
         <v>88</v>
       </c>
-      <c r="CM9" s="34">
+      <c r="CM9" s="33">
         <v>89</v>
       </c>
-      <c r="CN9" s="34">
+      <c r="CN9" s="33">
         <v>90</v>
       </c>
-      <c r="CO9" s="34">
+      <c r="CO9" s="33">
         <v>91</v>
       </c>
-      <c r="CP9" s="34">
+      <c r="CP9" s="33">
         <v>92</v>
       </c>
-      <c r="CQ9" s="34">
+      <c r="CQ9" s="33">
         <v>93</v>
       </c>
-      <c r="CR9" s="34">
+      <c r="CR9" s="33">
         <v>94</v>
       </c>
-      <c r="CS9" s="34">
+      <c r="CS9" s="33">
         <v>95</v>
       </c>
-      <c r="CT9" s="34">
+      <c r="CT9" s="33">
         <v>96</v>
       </c>
-      <c r="CU9" s="34">
+      <c r="CU9" s="33">
         <v>97</v>
       </c>
-      <c r="CV9" s="34">
+      <c r="CV9" s="33">
         <v>98</v>
       </c>
-      <c r="CW9" s="34">
+      <c r="CW9" s="33">
         <v>99</v>
       </c>
-      <c r="CX9" s="34">
+      <c r="CX9" s="33">
         <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:102" s="27" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="23" t="s">
+    <row r="11" spans="1:102" s="26" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="25"/>
-      <c r="R11" s="25"/>
-      <c r="S11" s="25"/>
-      <c r="T11" s="25"/>
-      <c r="U11" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="V11" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="W11" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="X11" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y11" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z11" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA11" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB11" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="AC11" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="AD11" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="AE11" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="AF11" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="AG11" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="AH11" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="AI11" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="AJ11" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="AK11" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="AL11" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="AM11" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="AN11" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="AO11" s="24" t="s">
+      <c r="B11" s="23"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24"/>
+      <c r="U11" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="V11" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="W11" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="X11" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y11" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z11" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA11" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB11" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC11" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD11" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE11" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF11" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG11" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH11" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI11" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AJ11" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AK11" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AL11" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AM11" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AN11" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="AO11" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="AP11" s="26" t="s">
+      <c r="AP11" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="AQ11" s="25"/>
-      <c r="AR11" s="25"/>
-      <c r="AS11" s="25"/>
-      <c r="AT11" s="25"/>
-      <c r="AU11" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="AV11" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="AW11" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="AX11" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="AY11" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="AZ11" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="BA11" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="BB11" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="BC11" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="BD11" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="BE11" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="BF11" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="BG11" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="BH11" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="BI11" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="BJ11" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="BK11" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="BL11" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="BM11" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="BN11" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="BO11" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="BP11" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="BQ11" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="BR11" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="BS11" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="BT11" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="BU11" s="25"/>
-      <c r="BV11" s="25"/>
-      <c r="BW11" s="25"/>
-      <c r="BX11" s="25"/>
-      <c r="BY11" s="25"/>
-      <c r="BZ11" s="24" t="s">
+      <c r="AQ11" s="24"/>
+      <c r="AR11" s="24"/>
+      <c r="AS11" s="24"/>
+      <c r="AT11" s="24"/>
+      <c r="AU11" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="AV11" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="AW11" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="AX11" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="AY11" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="AZ11" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="BA11" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="BB11" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="BC11" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="BD11" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="BE11" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="BF11" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="BG11" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="BH11" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="BI11" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="BJ11" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="BK11" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="BL11" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="BM11" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="BN11" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="BO11" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="BP11" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="BQ11" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="BR11" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="BS11" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="BT11" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="BU11" s="24"/>
+      <c r="BV11" s="24"/>
+      <c r="BW11" s="24"/>
+      <c r="BX11" s="24"/>
+      <c r="BY11" s="24"/>
+      <c r="BZ11" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="CA11" s="25" t="s">
+      <c r="CA11" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="CB11" s="25" t="s">
+      <c r="CB11" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="CC11" s="25" t="s">
+      <c r="CC11" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="CD11" s="25" t="s">
+      <c r="CD11" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="CE11" s="25" t="s">
+      <c r="CE11" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="CF11" s="25" t="s">
+      <c r="CF11" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="CG11" s="25" t="s">
+      <c r="CG11" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="CH11" s="25" t="s">
+      <c r="CH11" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="CI11" s="25" t="s">
+      <c r="CI11" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="CJ11" s="25" t="s">
+      <c r="CJ11" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="CK11" s="25" t="s">
+      <c r="CK11" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="CL11" s="25" t="s">
+      <c r="CL11" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="CM11" s="25" t="s">
+      <c r="CM11" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="CN11" s="25" t="s">
+      <c r="CN11" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="CO11" s="25" t="s">
+      <c r="CO11" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="CP11" s="25" t="s">
+      <c r="CP11" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="CQ11" s="25" t="s">
+      <c r="CQ11" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="CR11" s="25" t="s">
+      <c r="CR11" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="CS11" s="26" t="s">
+      <c r="CS11" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="CT11" s="24" t="s">
+      <c r="CT11" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="CU11" s="26" t="s">
+      <c r="CU11" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="CV11" s="25"/>
-      <c r="CW11" s="25"/>
-      <c r="CX11" s="25"/>
+      <c r="CV11" s="24"/>
+      <c r="CW11" s="24"/>
+      <c r="CX11" s="24"/>
     </row>
     <row r="12" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
@@ -1738,219 +1731,219 @@
     <row r="13" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:102" s="39" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="36" t="s">
+    <row r="14" spans="1:102" s="38" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="38" t="s">
+      <c r="B14" s="36"/>
+      <c r="C14" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="38" t="s">
+      <c r="D14" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="38" t="s">
+      <c r="E14" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="38" t="s">
+      <c r="F14" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="38" t="s">
+      <c r="G14" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="H14" s="38" t="s">
+      <c r="H14" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="I14" s="38" t="s">
+      <c r="I14" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="J14" s="38" t="s">
+      <c r="J14" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="K14" s="38" t="s">
+      <c r="K14" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="L14" s="38" t="s">
+      <c r="L14" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="M14" s="38" t="s">
+      <c r="M14" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="N14" s="38" t="s">
+      <c r="N14" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="O14" s="38" t="s">
+      <c r="O14" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="P14" s="38" t="s">
+      <c r="P14" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="Q14" s="38" t="s">
+      <c r="Q14" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="R14" s="38" t="s">
+      <c r="R14" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="S14" s="38" t="s">
+      <c r="S14" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="T14" s="38" t="s">
+      <c r="T14" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="U14" s="38" t="s">
+      <c r="U14" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="V14" s="38"/>
-      <c r="W14" s="38"/>
-      <c r="X14" s="38"/>
-      <c r="Y14" s="38" t="s">
+      <c r="V14" s="37"/>
+      <c r="W14" s="37"/>
+      <c r="X14" s="37"/>
+      <c r="Y14" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="Z14" s="38" t="s">
+      <c r="Z14" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="AA14" s="38" t="s">
+      <c r="AA14" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="AB14" s="38" t="s">
+      <c r="AB14" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="AC14" s="38" t="s">
+      <c r="AC14" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="AD14" s="38" t="s">
+      <c r="AD14" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="AE14" s="38" t="s">
+      <c r="AE14" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="AF14" s="38" t="s">
+      <c r="AF14" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="AG14" s="38" t="s">
+      <c r="AG14" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="AH14" s="38" t="s">
+      <c r="AH14" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="AI14" s="38"/>
-      <c r="AJ14" s="38"/>
-      <c r="AK14" s="38"/>
-      <c r="AL14" s="38"/>
-      <c r="AM14" s="38" t="s">
+      <c r="AI14" s="37"/>
+      <c r="AJ14" s="37"/>
+      <c r="AK14" s="37"/>
+      <c r="AL14" s="37"/>
+      <c r="AM14" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="AN14" s="38" t="s">
+      <c r="AN14" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="AO14" s="38" t="s">
+      <c r="AO14" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="AP14" s="38" t="s">
+      <c r="AP14" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="AQ14" s="38" t="s">
+      <c r="AQ14" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="AR14" s="38" t="s">
+      <c r="AR14" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="AS14" s="38" t="s">
+      <c r="AS14" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="AT14" s="38" t="s">
+      <c r="AT14" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="AU14" s="38"/>
-      <c r="AV14" s="38"/>
-      <c r="AW14" s="38"/>
-      <c r="AX14" s="38"/>
-      <c r="AY14" s="38" t="s">
+      <c r="AU14" s="37"/>
+      <c r="AV14" s="37"/>
+      <c r="AW14" s="37"/>
+      <c r="AX14" s="37"/>
+      <c r="AY14" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="AZ14" s="38" t="s">
+      <c r="AZ14" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="BA14" s="38" t="s">
+      <c r="BA14" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="BB14" s="38" t="s">
+      <c r="BB14" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="BC14" s="38" t="s">
+      <c r="BC14" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="BD14" s="38" t="s">
+      <c r="BD14" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="BE14" s="38"/>
-      <c r="BF14" s="38"/>
-      <c r="BG14" s="38"/>
-      <c r="BH14" s="38"/>
-      <c r="BI14" s="38"/>
-      <c r="BJ14" s="38" t="s">
+      <c r="BE14" s="37"/>
+      <c r="BF14" s="37"/>
+      <c r="BG14" s="37"/>
+      <c r="BH14" s="37"/>
+      <c r="BI14" s="37"/>
+      <c r="BJ14" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="BK14" s="38" t="s">
+      <c r="BK14" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="BL14" s="38" t="s">
+      <c r="BL14" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="BM14" s="38"/>
-      <c r="BN14" s="38"/>
-      <c r="BO14" s="38"/>
-      <c r="BP14" s="38"/>
-      <c r="BQ14" s="38"/>
-      <c r="BR14" s="38" t="s">
+      <c r="BM14" s="37"/>
+      <c r="BN14" s="37"/>
+      <c r="BO14" s="37"/>
+      <c r="BP14" s="37"/>
+      <c r="BQ14" s="37"/>
+      <c r="BR14" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="BS14" s="38" t="s">
+      <c r="BS14" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="BT14" s="38" t="s">
+      <c r="BT14" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="BU14" s="38" t="s">
+      <c r="BU14" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="BV14" s="38" t="s">
+      <c r="BV14" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="BW14" s="38" t="s">
+      <c r="BW14" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="BX14" s="38" t="s">
+      <c r="BX14" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="BY14" s="38" t="s">
+      <c r="BY14" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="BZ14" s="38"/>
-      <c r="CA14" s="38"/>
-      <c r="CB14" s="38"/>
-      <c r="CC14" s="38"/>
-      <c r="CD14" s="38"/>
-      <c r="CE14" s="38"/>
-      <c r="CF14" s="38"/>
-      <c r="CG14" s="38"/>
-      <c r="CH14" s="38"/>
-      <c r="CI14" s="38"/>
-      <c r="CJ14" s="38"/>
-      <c r="CK14" s="38"/>
-      <c r="CL14" s="38"/>
-      <c r="CM14" s="38"/>
-      <c r="CN14" s="38"/>
-      <c r="CO14" s="38"/>
-      <c r="CP14" s="38"/>
-      <c r="CQ14" s="38"/>
-      <c r="CR14" s="38"/>
-      <c r="CS14" s="38"/>
-      <c r="CT14" s="38"/>
-      <c r="CU14" s="38"/>
-      <c r="CV14" s="38"/>
-      <c r="CW14" s="38"/>
-      <c r="CX14" s="38"/>
+      <c r="BZ14" s="37"/>
+      <c r="CA14" s="37"/>
+      <c r="CB14" s="37"/>
+      <c r="CC14" s="37"/>
+      <c r="CD14" s="37"/>
+      <c r="CE14" s="37"/>
+      <c r="CF14" s="37"/>
+      <c r="CG14" s="37"/>
+      <c r="CH14" s="37"/>
+      <c r="CI14" s="37"/>
+      <c r="CJ14" s="37"/>
+      <c r="CK14" s="37"/>
+      <c r="CL14" s="37"/>
+      <c r="CM14" s="37"/>
+      <c r="CN14" s="37"/>
+      <c r="CO14" s="37"/>
+      <c r="CP14" s="37"/>
+      <c r="CQ14" s="37"/>
+      <c r="CR14" s="37"/>
+      <c r="CS14" s="37"/>
+      <c r="CT14" s="37"/>
+      <c r="CU14" s="37"/>
+      <c r="CV14" s="37"/>
+      <c r="CW14" s="37"/>
+      <c r="CX14" s="37"/>
     </row>
     <row r="15" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
@@ -1990,285 +1983,285 @@
       <c r="BD15" t="s">
         <v>30</v>
       </c>
-      <c r="BM15" s="22"/>
-      <c r="BN15" s="22"/>
-      <c r="BO15" s="22"/>
-      <c r="BP15" s="22"/>
-      <c r="BQ15" s="22"/>
-      <c r="BR15" s="22"/>
-      <c r="BS15" s="22"/>
-      <c r="BT15" s="22"/>
-      <c r="BU15" s="22"/>
-      <c r="BV15" s="22" t="s">
+      <c r="BM15" s="21"/>
+      <c r="BN15" s="21"/>
+      <c r="BO15" s="21"/>
+      <c r="BP15" s="21"/>
+      <c r="BQ15" s="21"/>
+      <c r="BR15" s="21"/>
+      <c r="BS15" s="21"/>
+      <c r="BT15" s="21"/>
+      <c r="BU15" s="21"/>
+      <c r="BV15" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="BW15" s="22"/>
-      <c r="BX15" s="22"/>
-      <c r="BY15" s="22"/>
-      <c r="BZ15" s="22"/>
-      <c r="CA15" s="22"/>
-      <c r="CB15" s="22"/>
-      <c r="CC15" s="22"/>
-      <c r="CD15" s="22"/>
-      <c r="CE15" s="22"/>
-      <c r="CF15" s="22"/>
-      <c r="CG15" s="22"/>
-      <c r="CH15" s="22"/>
-      <c r="CI15" s="22"/>
-      <c r="CJ15" s="22"/>
-      <c r="CK15" s="22"/>
-      <c r="CL15" s="22"/>
-      <c r="CM15" s="22"/>
-      <c r="CN15" s="22"/>
-      <c r="CO15" s="22"/>
+      <c r="BW15" s="21"/>
+      <c r="BX15" s="21"/>
+      <c r="BY15" s="21"/>
+      <c r="BZ15" s="21"/>
+      <c r="CA15" s="21"/>
+      <c r="CB15" s="21"/>
+      <c r="CC15" s="21"/>
+      <c r="CD15" s="21"/>
+      <c r="CE15" s="21"/>
+      <c r="CF15" s="21"/>
+      <c r="CG15" s="21"/>
+      <c r="CH15" s="21"/>
+      <c r="CI15" s="21"/>
+      <c r="CJ15" s="21"/>
+      <c r="CK15" s="21"/>
+      <c r="CL15" s="21"/>
+      <c r="CM15" s="21"/>
+      <c r="CN15" s="21"/>
+      <c r="CO15" s="21"/>
     </row>
     <row r="16" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
-      <c r="BM16" s="22"/>
-      <c r="BN16" s="22"/>
-      <c r="BO16" s="22"/>
-      <c r="BP16" s="22"/>
-      <c r="BQ16" s="22"/>
-      <c r="BR16" s="22"/>
-      <c r="BS16" s="22"/>
-      <c r="BT16" s="22"/>
-      <c r="BU16" s="22"/>
-      <c r="BV16" s="22"/>
-      <c r="BW16" s="22"/>
-      <c r="BX16" s="22"/>
-      <c r="BY16" s="22"/>
-      <c r="BZ16" s="22"/>
-      <c r="CA16" s="22"/>
-      <c r="CB16" s="22"/>
-      <c r="CC16" s="22"/>
-      <c r="CD16" s="22"/>
-      <c r="CE16" s="22"/>
-      <c r="CF16" s="22"/>
-      <c r="CG16" s="22"/>
-      <c r="CH16" s="22"/>
-      <c r="CI16" s="22"/>
-      <c r="CJ16" s="22"/>
-      <c r="CK16" s="22"/>
-      <c r="CL16" s="22"/>
-      <c r="CM16" s="22"/>
-      <c r="CN16" s="22"/>
-      <c r="CO16" s="22"/>
-    </row>
-    <row r="17" spans="1:102" s="32" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="28" t="s">
+      <c r="BM16" s="21"/>
+      <c r="BN16" s="21"/>
+      <c r="BO16" s="21"/>
+      <c r="BP16" s="21"/>
+      <c r="BQ16" s="21"/>
+      <c r="BR16" s="21"/>
+      <c r="BS16" s="21"/>
+      <c r="BT16" s="21"/>
+      <c r="BU16" s="21"/>
+      <c r="BV16" s="21"/>
+      <c r="BW16" s="21"/>
+      <c r="BX16" s="21"/>
+      <c r="BY16" s="21"/>
+      <c r="BZ16" s="21"/>
+      <c r="CA16" s="21"/>
+      <c r="CB16" s="21"/>
+      <c r="CC16" s="21"/>
+      <c r="CD16" s="21"/>
+      <c r="CE16" s="21"/>
+      <c r="CF16" s="21"/>
+      <c r="CG16" s="21"/>
+      <c r="CH16" s="21"/>
+      <c r="CI16" s="21"/>
+      <c r="CJ16" s="21"/>
+      <c r="CK16" s="21"/>
+      <c r="CL16" s="21"/>
+      <c r="CM16" s="21"/>
+      <c r="CN16" s="21"/>
+      <c r="CO16" s="21"/>
+    </row>
+    <row r="17" spans="1:102" s="31" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="M17" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="N17" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="O17" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="P17" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q17" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="R17" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="S17" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="T17" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="U17" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="V17" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="W17" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="X17" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y17" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z17" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA17" s="28" t="s">
+      <c r="B17" s="28"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="M17" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="N17" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="O17" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="P17" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q17" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="R17" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="S17" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="T17" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="U17" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="V17" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="W17" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="X17" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y17" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z17" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA17" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="AB17" s="30"/>
-      <c r="AC17" s="30"/>
-      <c r="AD17" s="30"/>
-      <c r="AE17" s="30"/>
-      <c r="AF17" s="30"/>
-      <c r="AG17" s="30"/>
-      <c r="AH17" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="AI17" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="AJ17" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="AK17" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="AL17" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="AM17" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="AN17" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="AO17" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="AP17" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="AQ17" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="AR17" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="AS17" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="AT17" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="AU17" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="AV17" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="AW17" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="AX17" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="AY17" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="AZ17" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="BA17" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="BB17" s="29" t="s">
+      <c r="AB17" s="29"/>
+      <c r="AC17" s="29"/>
+      <c r="AD17" s="29"/>
+      <c r="AE17" s="29"/>
+      <c r="AF17" s="29"/>
+      <c r="AG17" s="29"/>
+      <c r="AH17" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="AI17" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ17" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK17" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AL17" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM17" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AN17" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO17" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AP17" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AQ17" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AR17" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AS17" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AT17" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU17" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV17" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AW17" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AX17" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY17" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ17" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="BA17" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="BB17" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="BC17" s="31" t="s">
+      <c r="BC17" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="BD17" s="30"/>
-      <c r="BE17" s="30"/>
-      <c r="BF17" s="30"/>
-      <c r="BG17" s="30"/>
-      <c r="BH17" s="30"/>
-      <c r="BI17" s="30"/>
-      <c r="BJ17" s="30"/>
-      <c r="BK17" s="30"/>
-      <c r="BL17" s="30"/>
-      <c r="BM17" s="30"/>
-      <c r="BN17" s="29" t="s">
+      <c r="BD17" s="29"/>
+      <c r="BE17" s="29"/>
+      <c r="BF17" s="29"/>
+      <c r="BG17" s="29"/>
+      <c r="BH17" s="29"/>
+      <c r="BI17" s="29"/>
+      <c r="BJ17" s="29"/>
+      <c r="BK17" s="29"/>
+      <c r="BL17" s="29"/>
+      <c r="BM17" s="29"/>
+      <c r="BN17" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="BO17" s="30" t="s">
+      <c r="BO17" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BP17" s="30" t="s">
+      <c r="BP17" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BQ17" s="30" t="s">
+      <c r="BQ17" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BR17" s="30" t="s">
+      <c r="BR17" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BS17" s="30" t="s">
+      <c r="BS17" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BT17" s="30" t="s">
+      <c r="BT17" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BU17" s="30" t="s">
+      <c r="BU17" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BV17" s="30" t="s">
+      <c r="BV17" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BW17" s="30" t="s">
+      <c r="BW17" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BX17" s="30" t="s">
+      <c r="BX17" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BY17" s="30" t="s">
+      <c r="BY17" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="BZ17" s="30" t="s">
+      <c r="BZ17" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="CA17" s="30" t="s">
+      <c r="CA17" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="CB17" s="30" t="s">
+      <c r="CB17" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="CC17" s="31" t="s">
+      <c r="CC17" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="CD17" s="28" t="s">
+      <c r="CD17" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="CE17" s="30"/>
-      <c r="CF17" s="30"/>
-      <c r="CG17" s="30"/>
-      <c r="CH17" s="30"/>
-      <c r="CI17" s="30"/>
-      <c r="CJ17" s="30"/>
-      <c r="CK17" s="30"/>
-      <c r="CL17" s="30"/>
-      <c r="CM17" s="30"/>
-      <c r="CN17" s="30"/>
-      <c r="CO17" s="30"/>
-      <c r="CP17" s="30"/>
-      <c r="CQ17" s="30"/>
-      <c r="CR17" s="30"/>
-      <c r="CS17" s="30"/>
-      <c r="CT17" s="30"/>
-      <c r="CU17" s="30"/>
-      <c r="CV17" s="30"/>
-      <c r="CW17" s="30"/>
-      <c r="CX17" s="30"/>
+      <c r="CE17" s="29"/>
+      <c r="CF17" s="29"/>
+      <c r="CG17" s="29"/>
+      <c r="CH17" s="29"/>
+      <c r="CI17" s="29"/>
+      <c r="CJ17" s="29"/>
+      <c r="CK17" s="29"/>
+      <c r="CL17" s="29"/>
+      <c r="CM17" s="29"/>
+      <c r="CN17" s="29"/>
+      <c r="CO17" s="29"/>
+      <c r="CP17" s="29"/>
+      <c r="CQ17" s="29"/>
+      <c r="CR17" s="29"/>
+      <c r="CS17" s="29"/>
+      <c r="CT17" s="29"/>
+      <c r="CU17" s="29"/>
+      <c r="CV17" s="29"/>
+      <c r="CW17" s="29"/>
+      <c r="CX17" s="29"/>
     </row>
     <row r="18" spans="1:102" x14ac:dyDescent="0.3">
       <c r="L18" s="13" t="s">
@@ -2376,147 +2369,147 @@
       <c r="BA18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="BM18" s="22"/>
-      <c r="BN18" s="22" t="s">
+      <c r="BM18" s="21"/>
+      <c r="BN18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="BO18" s="22" t="s">
+      <c r="BO18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="BP18" s="22" t="s">
+      <c r="BP18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="BQ18" s="22" t="s">
+      <c r="BQ18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="BR18" s="22" t="s">
+      <c r="BR18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="BS18" s="22" t="s">
+      <c r="BS18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="BT18" s="22" t="s">
+      <c r="BT18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="BU18" s="22" t="s">
+      <c r="BU18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="BV18" s="22" t="s">
+      <c r="BV18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="BW18" s="22" t="s">
+      <c r="BW18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="BX18" s="22" t="s">
+      <c r="BX18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="BY18" s="22" t="s">
+      <c r="BY18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="BZ18" s="22" t="s">
+      <c r="BZ18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="CA18" s="22" t="s">
+      <c r="CA18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="CB18" s="22" t="s">
+      <c r="CB18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="CC18" s="22" t="s">
+      <c r="CC18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="CD18" s="22"/>
-      <c r="CE18" s="22"/>
-      <c r="CF18" s="22"/>
-      <c r="CG18" s="22"/>
-      <c r="CH18" s="22"/>
-      <c r="CI18" s="22"/>
-      <c r="CJ18" s="22"/>
-      <c r="CK18" s="22"/>
-      <c r="CL18" s="22"/>
-      <c r="CM18" s="22"/>
-      <c r="CN18" s="22"/>
-      <c r="CO18" s="22"/>
+      <c r="CD18" s="21"/>
+      <c r="CE18" s="21"/>
+      <c r="CF18" s="21"/>
+      <c r="CG18" s="21"/>
+      <c r="CH18" s="21"/>
+      <c r="CI18" s="21"/>
+      <c r="CJ18" s="21"/>
+      <c r="CK18" s="21"/>
+      <c r="CL18" s="21"/>
+      <c r="CM18" s="21"/>
+      <c r="CN18" s="21"/>
+      <c r="CO18" s="21"/>
     </row>
     <row r="19" spans="1:102" x14ac:dyDescent="0.3">
-      <c r="BZ19" s="22"/>
-      <c r="CA19" s="22"/>
-      <c r="CB19" s="22"/>
-      <c r="CC19" s="22"/>
-      <c r="CD19" s="22"/>
-      <c r="CE19" s="22"/>
-      <c r="CF19" s="22"/>
-      <c r="CG19" s="22"/>
-      <c r="CH19" s="22"/>
-      <c r="CI19" s="22"/>
-      <c r="CJ19" s="22"/>
-      <c r="CK19" s="22"/>
-      <c r="CL19" s="22"/>
-      <c r="CM19" s="22"/>
-      <c r="CN19" s="22"/>
-      <c r="CO19" s="22"/>
+      <c r="BZ19" s="21"/>
+      <c r="CA19" s="21"/>
+      <c r="CB19" s="21"/>
+      <c r="CC19" s="21"/>
+      <c r="CD19" s="21"/>
+      <c r="CE19" s="21"/>
+      <c r="CF19" s="21"/>
+      <c r="CG19" s="21"/>
+      <c r="CH19" s="21"/>
+      <c r="CI19" s="21"/>
+      <c r="CJ19" s="21"/>
+      <c r="CK19" s="21"/>
+      <c r="CL19" s="21"/>
+      <c r="CM19" s="21"/>
+      <c r="CN19" s="21"/>
+      <c r="CO19" s="21"/>
     </row>
     <row r="20" spans="1:102" x14ac:dyDescent="0.3">
-      <c r="BM20" s="22"/>
-      <c r="BN20" s="22"/>
-      <c r="BO20" s="22"/>
-      <c r="BP20" s="22"/>
-      <c r="BQ20" s="22"/>
-      <c r="BR20" s="22"/>
-      <c r="BS20" s="22"/>
-      <c r="BT20" s="22"/>
-      <c r="BU20" s="22"/>
-      <c r="BV20" s="22"/>
-      <c r="BW20" s="22"/>
-      <c r="BX20" s="22"/>
-      <c r="BY20" s="22"/>
-      <c r="BZ20" s="22"/>
-      <c r="CA20" s="22"/>
-      <c r="CB20" s="22"/>
-      <c r="CC20" s="22"/>
-      <c r="CD20" s="22"/>
-      <c r="CE20" s="22"/>
-      <c r="CF20" s="22"/>
-      <c r="CG20" s="22"/>
-      <c r="CH20" s="22"/>
-      <c r="CI20" s="22"/>
-      <c r="CJ20" s="22"/>
-      <c r="CK20" s="22"/>
-      <c r="CL20" s="22"/>
-      <c r="CM20" s="22"/>
-      <c r="CN20" s="22"/>
-      <c r="CO20" s="22"/>
+      <c r="BM20" s="21"/>
+      <c r="BN20" s="21"/>
+      <c r="BO20" s="21"/>
+      <c r="BP20" s="21"/>
+      <c r="BQ20" s="21"/>
+      <c r="BR20" s="21"/>
+      <c r="BS20" s="21"/>
+      <c r="BT20" s="21"/>
+      <c r="BU20" s="21"/>
+      <c r="BV20" s="21"/>
+      <c r="BW20" s="21"/>
+      <c r="BX20" s="21"/>
+      <c r="BY20" s="21"/>
+      <c r="BZ20" s="21"/>
+      <c r="CA20" s="21"/>
+      <c r="CB20" s="21"/>
+      <c r="CC20" s="21"/>
+      <c r="CD20" s="21"/>
+      <c r="CE20" s="21"/>
+      <c r="CF20" s="21"/>
+      <c r="CG20" s="21"/>
+      <c r="CH20" s="21"/>
+      <c r="CI20" s="21"/>
+      <c r="CJ20" s="21"/>
+      <c r="CK20" s="21"/>
+      <c r="CL20" s="21"/>
+      <c r="CM20" s="21"/>
+      <c r="CN20" s="21"/>
+      <c r="CO20" s="21"/>
     </row>
     <row r="21" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="BM21" s="22"/>
-      <c r="BN21" s="22"/>
-      <c r="BO21" s="22"/>
-      <c r="BP21" s="22"/>
-      <c r="BQ21" s="22"/>
-      <c r="BR21" s="22"/>
-      <c r="BS21" s="22"/>
-      <c r="BT21" s="22"/>
-      <c r="BU21" s="22"/>
-      <c r="BV21" s="22"/>
-      <c r="BW21" s="22"/>
-      <c r="BX21" s="22"/>
-      <c r="BY21" s="22"/>
-      <c r="BZ21" s="22"/>
-      <c r="CA21" s="22"/>
-      <c r="CB21" s="22"/>
-      <c r="CC21" s="22"/>
-      <c r="CD21" s="22"/>
-      <c r="CE21" s="22"/>
-      <c r="CF21" s="22"/>
-      <c r="CG21" s="22"/>
-      <c r="CH21" s="22"/>
-      <c r="CI21" s="22"/>
-      <c r="CJ21" s="22"/>
-      <c r="CK21" s="22"/>
-      <c r="CL21" s="22"/>
-      <c r="CM21" s="22"/>
-      <c r="CN21" s="22"/>
-      <c r="CO21" s="22"/>
+      <c r="BM21" s="21"/>
+      <c r="BN21" s="21"/>
+      <c r="BO21" s="21"/>
+      <c r="BP21" s="21"/>
+      <c r="BQ21" s="21"/>
+      <c r="BR21" s="21"/>
+      <c r="BS21" s="21"/>
+      <c r="BT21" s="21"/>
+      <c r="BU21" s="21"/>
+      <c r="BV21" s="21"/>
+      <c r="BW21" s="21"/>
+      <c r="BX21" s="21"/>
+      <c r="BY21" s="21"/>
+      <c r="BZ21" s="21"/>
+      <c r="CA21" s="21"/>
+      <c r="CB21" s="21"/>
+      <c r="CC21" s="21"/>
+      <c r="CD21" s="21"/>
+      <c r="CE21" s="21"/>
+      <c r="CF21" s="21"/>
+      <c r="CG21" s="21"/>
+      <c r="CH21" s="21"/>
+      <c r="CI21" s="21"/>
+      <c r="CJ21" s="21"/>
+      <c r="CK21" s="21"/>
+      <c r="CL21" s="21"/>
+      <c r="CM21" s="21"/>
+      <c r="CN21" s="21"/>
+      <c r="CO21" s="21"/>
     </row>
     <row r="22" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="19" t="s">
@@ -2546,35 +2539,35 @@
       <c r="P22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="BM22" s="22"/>
-      <c r="BN22" s="22"/>
-      <c r="BO22" s="22"/>
-      <c r="BP22" s="22"/>
-      <c r="BQ22" s="22"/>
-      <c r="BR22" s="22"/>
-      <c r="BS22" s="22"/>
-      <c r="BT22" s="22"/>
-      <c r="BU22" s="22"/>
-      <c r="BV22" s="22"/>
-      <c r="BW22" s="22"/>
-      <c r="BX22" s="22"/>
-      <c r="BY22" s="22"/>
-      <c r="BZ22" s="22"/>
-      <c r="CA22" s="22"/>
-      <c r="CB22" s="22"/>
-      <c r="CC22" s="22"/>
-      <c r="CD22" s="22"/>
-      <c r="CE22" s="22"/>
-      <c r="CF22" s="22"/>
-      <c r="CG22" s="22"/>
-      <c r="CH22" s="22"/>
-      <c r="CI22" s="22"/>
-      <c r="CJ22" s="22"/>
-      <c r="CK22" s="22"/>
-      <c r="CL22" s="22"/>
-      <c r="CM22" s="22"/>
-      <c r="CN22" s="22"/>
-      <c r="CO22" s="22"/>
+      <c r="BM22" s="21"/>
+      <c r="BN22" s="21"/>
+      <c r="BO22" s="21"/>
+      <c r="BP22" s="21"/>
+      <c r="BQ22" s="21"/>
+      <c r="BR22" s="21"/>
+      <c r="BS22" s="21"/>
+      <c r="BT22" s="21"/>
+      <c r="BU22" s="21"/>
+      <c r="BV22" s="21"/>
+      <c r="BW22" s="21"/>
+      <c r="BX22" s="21"/>
+      <c r="BY22" s="21"/>
+      <c r="BZ22" s="21"/>
+      <c r="CA22" s="21"/>
+      <c r="CB22" s="21"/>
+      <c r="CC22" s="21"/>
+      <c r="CD22" s="21"/>
+      <c r="CE22" s="21"/>
+      <c r="CF22" s="21"/>
+      <c r="CG22" s="21"/>
+      <c r="CH22" s="21"/>
+      <c r="CI22" s="21"/>
+      <c r="CJ22" s="21"/>
+      <c r="CK22" s="21"/>
+      <c r="CL22" s="21"/>
+      <c r="CM22" s="21"/>
+      <c r="CN22" s="21"/>
+      <c r="CO22" s="21"/>
     </row>
     <row r="23" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="L23" s="1" t="s">
@@ -2586,35 +2579,35 @@
       <c r="P23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="BM23" s="22"/>
-      <c r="BN23" s="22"/>
-      <c r="BO23" s="22"/>
-      <c r="BP23" s="22"/>
-      <c r="BQ23" s="22"/>
-      <c r="BR23" s="22"/>
-      <c r="BS23" s="22"/>
-      <c r="BT23" s="22"/>
-      <c r="BU23" s="22"/>
-      <c r="BV23" s="22"/>
-      <c r="BW23" s="22"/>
-      <c r="BX23" s="22"/>
-      <c r="BY23" s="22"/>
-      <c r="BZ23" s="22"/>
-      <c r="CA23" s="22"/>
-      <c r="CB23" s="22"/>
-      <c r="CC23" s="22"/>
-      <c r="CD23" s="22"/>
-      <c r="CE23" s="22"/>
-      <c r="CF23" s="22"/>
-      <c r="CG23" s="22"/>
-      <c r="CH23" s="22"/>
-      <c r="CI23" s="22"/>
-      <c r="CJ23" s="22"/>
-      <c r="CK23" s="22"/>
-      <c r="CL23" s="22"/>
-      <c r="CM23" s="22"/>
-      <c r="CN23" s="22"/>
-      <c r="CO23" s="22"/>
+      <c r="BM23" s="21"/>
+      <c r="BN23" s="21"/>
+      <c r="BO23" s="21"/>
+      <c r="BP23" s="21"/>
+      <c r="BQ23" s="21"/>
+      <c r="BR23" s="21"/>
+      <c r="BS23" s="21"/>
+      <c r="BT23" s="21"/>
+      <c r="BU23" s="21"/>
+      <c r="BV23" s="21"/>
+      <c r="BW23" s="21"/>
+      <c r="BX23" s="21"/>
+      <c r="BY23" s="21"/>
+      <c r="BZ23" s="21"/>
+      <c r="CA23" s="21"/>
+      <c r="CB23" s="21"/>
+      <c r="CC23" s="21"/>
+      <c r="CD23" s="21"/>
+      <c r="CE23" s="21"/>
+      <c r="CF23" s="21"/>
+      <c r="CG23" s="21"/>
+      <c r="CH23" s="21"/>
+      <c r="CI23" s="21"/>
+      <c r="CJ23" s="21"/>
+      <c r="CK23" s="21"/>
+      <c r="CL23" s="21"/>
+      <c r="CM23" s="21"/>
+      <c r="CN23" s="21"/>
+      <c r="CO23" s="21"/>
     </row>
     <row r="24" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
@@ -2638,35 +2631,35 @@
       <c r="G24" s="10">
         <v>6</v>
       </c>
-      <c r="BM24" s="22"/>
-      <c r="BN24" s="22"/>
-      <c r="BO24" s="22"/>
-      <c r="BP24" s="22"/>
-      <c r="BQ24" s="22"/>
-      <c r="BR24" s="22"/>
-      <c r="BS24" s="22"/>
-      <c r="BT24" s="22"/>
-      <c r="BU24" s="22"/>
-      <c r="BV24" s="22"/>
-      <c r="BW24" s="22"/>
-      <c r="BX24" s="22"/>
-      <c r="BY24" s="22"/>
-      <c r="BZ24" s="22"/>
-      <c r="CA24" s="22"/>
-      <c r="CB24" s="22"/>
-      <c r="CC24" s="22"/>
-      <c r="CD24" s="22"/>
-      <c r="CE24" s="22"/>
-      <c r="CF24" s="22"/>
-      <c r="CG24" s="22"/>
-      <c r="CH24" s="22"/>
-      <c r="CI24" s="22"/>
-      <c r="CJ24" s="22"/>
-      <c r="CK24" s="22"/>
-      <c r="CL24" s="22"/>
-      <c r="CM24" s="22"/>
-      <c r="CN24" s="22"/>
-      <c r="CO24" s="22"/>
+      <c r="BM24" s="21"/>
+      <c r="BN24" s="21"/>
+      <c r="BO24" s="21"/>
+      <c r="BP24" s="21"/>
+      <c r="BQ24" s="21"/>
+      <c r="BR24" s="21"/>
+      <c r="BS24" s="21"/>
+      <c r="BT24" s="21"/>
+      <c r="BU24" s="21"/>
+      <c r="BV24" s="21"/>
+      <c r="BW24" s="21"/>
+      <c r="BX24" s="21"/>
+      <c r="BY24" s="21"/>
+      <c r="BZ24" s="21"/>
+      <c r="CA24" s="21"/>
+      <c r="CB24" s="21"/>
+      <c r="CC24" s="21"/>
+      <c r="CD24" s="21"/>
+      <c r="CE24" s="21"/>
+      <c r="CF24" s="21"/>
+      <c r="CG24" s="21"/>
+      <c r="CH24" s="21"/>
+      <c r="CI24" s="21"/>
+      <c r="CJ24" s="21"/>
+      <c r="CK24" s="21"/>
+      <c r="CL24" s="21"/>
+      <c r="CM24" s="21"/>
+      <c r="CN24" s="21"/>
+      <c r="CO24" s="21"/>
     </row>
     <row r="25" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
@@ -2714,35 +2707,35 @@
       <c r="P25" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="BM25" s="22"/>
-      <c r="BN25" s="22"/>
-      <c r="BO25" s="22"/>
-      <c r="BP25" s="22"/>
-      <c r="BQ25" s="22"/>
-      <c r="BR25" s="22"/>
-      <c r="BS25" s="22"/>
-      <c r="BT25" s="22"/>
-      <c r="BU25" s="22"/>
-      <c r="BV25" s="22"/>
-      <c r="BW25" s="22"/>
-      <c r="BX25" s="22"/>
-      <c r="BY25" s="22"/>
-      <c r="BZ25" s="22"/>
-      <c r="CA25" s="22"/>
-      <c r="CB25" s="22"/>
-      <c r="CC25" s="22"/>
-      <c r="CD25" s="22"/>
-      <c r="CE25" s="22"/>
-      <c r="CF25" s="22"/>
-      <c r="CG25" s="22"/>
-      <c r="CH25" s="22"/>
-      <c r="CI25" s="22"/>
-      <c r="CJ25" s="22"/>
-      <c r="CK25" s="22"/>
-      <c r="CL25" s="22"/>
-      <c r="CM25" s="22"/>
-      <c r="CN25" s="22"/>
-      <c r="CO25" s="22"/>
+      <c r="BM25" s="21"/>
+      <c r="BN25" s="21"/>
+      <c r="BO25" s="21"/>
+      <c r="BP25" s="21"/>
+      <c r="BQ25" s="21"/>
+      <c r="BR25" s="21"/>
+      <c r="BS25" s="21"/>
+      <c r="BT25" s="21"/>
+      <c r="BU25" s="21"/>
+      <c r="BV25" s="21"/>
+      <c r="BW25" s="21"/>
+      <c r="BX25" s="21"/>
+      <c r="BY25" s="21"/>
+      <c r="BZ25" s="21"/>
+      <c r="CA25" s="21"/>
+      <c r="CB25" s="21"/>
+      <c r="CC25" s="21"/>
+      <c r="CD25" s="21"/>
+      <c r="CE25" s="21"/>
+      <c r="CF25" s="21"/>
+      <c r="CG25" s="21"/>
+      <c r="CH25" s="21"/>
+      <c r="CI25" s="21"/>
+      <c r="CJ25" s="21"/>
+      <c r="CK25" s="21"/>
+      <c r="CL25" s="21"/>
+      <c r="CM25" s="21"/>
+      <c r="CN25" s="21"/>
+      <c r="CO25" s="21"/>
     </row>
     <row r="26" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A26" s="14" t="s">
@@ -2775,35 +2768,35 @@
       <c r="P26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="BM26" s="22"/>
-      <c r="BN26" s="22"/>
-      <c r="BO26" s="22"/>
-      <c r="BP26" s="22"/>
-      <c r="BQ26" s="22"/>
-      <c r="BR26" s="22"/>
-      <c r="BS26" s="22"/>
-      <c r="BT26" s="22"/>
-      <c r="BU26" s="22"/>
-      <c r="BV26" s="22"/>
-      <c r="BW26" s="22"/>
-      <c r="BX26" s="22"/>
-      <c r="BY26" s="22"/>
-      <c r="BZ26" s="22"/>
-      <c r="CA26" s="22"/>
-      <c r="CB26" s="22"/>
-      <c r="CC26" s="22"/>
-      <c r="CD26" s="22"/>
-      <c r="CE26" s="22"/>
-      <c r="CF26" s="22"/>
-      <c r="CG26" s="22"/>
-      <c r="CH26" s="22"/>
-      <c r="CI26" s="22"/>
-      <c r="CJ26" s="22"/>
-      <c r="CK26" s="22"/>
-      <c r="CL26" s="22"/>
-      <c r="CM26" s="22"/>
-      <c r="CN26" s="22"/>
-      <c r="CO26" s="22"/>
+      <c r="BM26" s="21"/>
+      <c r="BN26" s="21"/>
+      <c r="BO26" s="21"/>
+      <c r="BP26" s="21"/>
+      <c r="BQ26" s="21"/>
+      <c r="BR26" s="21"/>
+      <c r="BS26" s="21"/>
+      <c r="BT26" s="21"/>
+      <c r="BU26" s="21"/>
+      <c r="BV26" s="21"/>
+      <c r="BW26" s="21"/>
+      <c r="BX26" s="21"/>
+      <c r="BY26" s="21"/>
+      <c r="BZ26" s="21"/>
+      <c r="CA26" s="21"/>
+      <c r="CB26" s="21"/>
+      <c r="CC26" s="21"/>
+      <c r="CD26" s="21"/>
+      <c r="CE26" s="21"/>
+      <c r="CF26" s="21"/>
+      <c r="CG26" s="21"/>
+      <c r="CH26" s="21"/>
+      <c r="CI26" s="21"/>
+      <c r="CJ26" s="21"/>
+      <c r="CK26" s="21"/>
+      <c r="CL26" s="21"/>
+      <c r="CM26" s="21"/>
+      <c r="CN26" s="21"/>
+      <c r="CO26" s="21"/>
     </row>
     <row r="27" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
@@ -2822,35 +2815,35 @@
       <c r="L27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="BM27" s="22"/>
-      <c r="BN27" s="22"/>
-      <c r="BO27" s="22"/>
-      <c r="BP27" s="22"/>
-      <c r="BQ27" s="22"/>
-      <c r="BR27" s="22"/>
-      <c r="BS27" s="22"/>
-      <c r="BT27" s="22"/>
-      <c r="BU27" s="22"/>
-      <c r="BV27" s="22"/>
-      <c r="BW27" s="22"/>
-      <c r="BX27" s="22"/>
-      <c r="BY27" s="22"/>
-      <c r="BZ27" s="22"/>
-      <c r="CA27" s="22"/>
-      <c r="CB27" s="22"/>
-      <c r="CC27" s="22"/>
-      <c r="CD27" s="22"/>
-      <c r="CE27" s="22"/>
-      <c r="CF27" s="22"/>
-      <c r="CG27" s="22"/>
-      <c r="CH27" s="22"/>
-      <c r="CI27" s="22"/>
-      <c r="CJ27" s="22"/>
-      <c r="CK27" s="22"/>
-      <c r="CL27" s="22"/>
-      <c r="CM27" s="22"/>
-      <c r="CN27" s="22"/>
-      <c r="CO27" s="22"/>
+      <c r="BM27" s="21"/>
+      <c r="BN27" s="21"/>
+      <c r="BO27" s="21"/>
+      <c r="BP27" s="21"/>
+      <c r="BQ27" s="21"/>
+      <c r="BR27" s="21"/>
+      <c r="BS27" s="21"/>
+      <c r="BT27" s="21"/>
+      <c r="BU27" s="21"/>
+      <c r="BV27" s="21"/>
+      <c r="BW27" s="21"/>
+      <c r="BX27" s="21"/>
+      <c r="BY27" s="21"/>
+      <c r="BZ27" s="21"/>
+      <c r="CA27" s="21"/>
+      <c r="CB27" s="21"/>
+      <c r="CC27" s="21"/>
+      <c r="CD27" s="21"/>
+      <c r="CE27" s="21"/>
+      <c r="CF27" s="21"/>
+      <c r="CG27" s="21"/>
+      <c r="CH27" s="21"/>
+      <c r="CI27" s="21"/>
+      <c r="CJ27" s="21"/>
+      <c r="CK27" s="21"/>
+      <c r="CL27" s="21"/>
+      <c r="CM27" s="21"/>
+      <c r="CN27" s="21"/>
+      <c r="CO27" s="21"/>
     </row>
     <row r="28" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
@@ -3015,67 +3008,67 @@
       <c r="BB28" s="4">
         <v>52</v>
       </c>
-      <c r="BM28" s="22"/>
-      <c r="BN28" s="22"/>
-      <c r="BO28" s="22"/>
-      <c r="BP28" s="22"/>
-      <c r="BQ28" s="22"/>
-      <c r="BR28" s="22"/>
-      <c r="BS28" s="22"/>
-      <c r="BT28" s="22"/>
-      <c r="BU28" s="22"/>
-      <c r="BV28" s="22"/>
-      <c r="BW28" s="22"/>
-      <c r="BX28" s="22"/>
-      <c r="BY28" s="22"/>
-      <c r="BZ28" s="22"/>
-      <c r="CA28" s="22"/>
-      <c r="CB28" s="22"/>
-      <c r="CC28" s="22"/>
-      <c r="CD28" s="22"/>
-      <c r="CE28" s="22"/>
-      <c r="CF28" s="22"/>
-      <c r="CG28" s="22"/>
-      <c r="CH28" s="22"/>
-      <c r="CI28" s="22"/>
-      <c r="CJ28" s="22"/>
-      <c r="CK28" s="22"/>
-      <c r="CL28" s="22"/>
-      <c r="CM28" s="22"/>
-      <c r="CN28" s="22"/>
-      <c r="CO28" s="22"/>
+      <c r="BM28" s="21"/>
+      <c r="BN28" s="21"/>
+      <c r="BO28" s="21"/>
+      <c r="BP28" s="21"/>
+      <c r="BQ28" s="21"/>
+      <c r="BR28" s="21"/>
+      <c r="BS28" s="21"/>
+      <c r="BT28" s="21"/>
+      <c r="BU28" s="21"/>
+      <c r="BV28" s="21"/>
+      <c r="BW28" s="21"/>
+      <c r="BX28" s="21"/>
+      <c r="BY28" s="21"/>
+      <c r="BZ28" s="21"/>
+      <c r="CA28" s="21"/>
+      <c r="CB28" s="21"/>
+      <c r="CC28" s="21"/>
+      <c r="CD28" s="21"/>
+      <c r="CE28" s="21"/>
+      <c r="CF28" s="21"/>
+      <c r="CG28" s="21"/>
+      <c r="CH28" s="21"/>
+      <c r="CI28" s="21"/>
+      <c r="CJ28" s="21"/>
+      <c r="CK28" s="21"/>
+      <c r="CL28" s="21"/>
+      <c r="CM28" s="21"/>
+      <c r="CN28" s="21"/>
+      <c r="CO28" s="21"/>
     </row>
     <row r="29" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
-      <c r="BM29" s="22"/>
-      <c r="BN29" s="22"/>
-      <c r="BO29" s="22"/>
-      <c r="BP29" s="22"/>
-      <c r="BQ29" s="22"/>
-      <c r="BR29" s="22"/>
-      <c r="BS29" s="22"/>
-      <c r="BT29" s="22"/>
-      <c r="BU29" s="22"/>
-      <c r="BV29" s="22"/>
-      <c r="BW29" s="22"/>
-      <c r="BX29" s="22"/>
-      <c r="BY29" s="22"/>
-      <c r="BZ29" s="22"/>
-      <c r="CA29" s="22"/>
-      <c r="CB29" s="22"/>
-      <c r="CC29" s="22"/>
-      <c r="CD29" s="22"/>
-      <c r="CE29" s="22"/>
-      <c r="CF29" s="22"/>
-      <c r="CG29" s="22"/>
-      <c r="CH29" s="22"/>
-      <c r="CI29" s="22"/>
-      <c r="CJ29" s="22"/>
-      <c r="CK29" s="22"/>
-      <c r="CL29" s="22"/>
-      <c r="CM29" s="22"/>
-      <c r="CN29" s="22"/>
-      <c r="CO29" s="22"/>
+      <c r="BM29" s="21"/>
+      <c r="BN29" s="21"/>
+      <c r="BO29" s="21"/>
+      <c r="BP29" s="21"/>
+      <c r="BQ29" s="21"/>
+      <c r="BR29" s="21"/>
+      <c r="BS29" s="21"/>
+      <c r="BT29" s="21"/>
+      <c r="BU29" s="21"/>
+      <c r="BV29" s="21"/>
+      <c r="BW29" s="21"/>
+      <c r="BX29" s="21"/>
+      <c r="BY29" s="21"/>
+      <c r="BZ29" s="21"/>
+      <c r="CA29" s="21"/>
+      <c r="CB29" s="21"/>
+      <c r="CC29" s="21"/>
+      <c r="CD29" s="21"/>
+      <c r="CE29" s="21"/>
+      <c r="CF29" s="21"/>
+      <c r="CG29" s="21"/>
+      <c r="CH29" s="21"/>
+      <c r="CI29" s="21"/>
+      <c r="CJ29" s="21"/>
+      <c r="CK29" s="21"/>
+      <c r="CL29" s="21"/>
+      <c r="CM29" s="21"/>
+      <c r="CN29" s="21"/>
+      <c r="CO29" s="21"/>
     </row>
     <row r="30" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
@@ -3092,11 +3085,19 @@
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-      <c r="P30" s="4"/>
-      <c r="Q30" s="5" t="s">
+      <c r="M30" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q30" s="4" t="s">
         <v>20</v>
       </c>
       <c r="R30" s="4" t="s">
@@ -3141,28 +3142,15 @@
       <c r="AE30" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AF30" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="AG30" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="AH30" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="AI30" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="AJ30" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="AK30" s="5" t="s">
+      <c r="AF30" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG30" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="AL30" s="6" t="s">
+      <c r="AH30" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="AM30" s="4"/>
       <c r="AN30" s="4"/>
       <c r="AO30" s="4"/>
       <c r="AP30" s="4"/>
@@ -3178,99 +3166,159 @@
       <c r="AZ30" s="4"/>
       <c r="BA30" s="4"/>
       <c r="BB30" s="4"/>
-      <c r="BM30" s="22"/>
-      <c r="BN30" s="22"/>
-      <c r="BO30" s="22"/>
-      <c r="BP30" s="22"/>
-      <c r="BQ30" s="22"/>
-      <c r="BR30" s="22"/>
-      <c r="BS30" s="22"/>
-      <c r="BT30" s="22"/>
-      <c r="BU30" s="22"/>
-      <c r="BV30" s="22"/>
-      <c r="BW30" s="22"/>
-      <c r="BX30" s="22"/>
-      <c r="BY30" s="22"/>
-      <c r="BZ30" s="22"/>
-      <c r="CA30" s="22"/>
-      <c r="CB30" s="22"/>
-      <c r="CC30" s="22"/>
-      <c r="CD30" s="22"/>
-      <c r="CE30" s="22"/>
-      <c r="CF30" s="22"/>
-      <c r="CG30" s="22"/>
-      <c r="CH30" s="22"/>
-      <c r="CI30" s="22"/>
-      <c r="CJ30" s="22"/>
-      <c r="CK30" s="22"/>
-      <c r="CL30" s="22"/>
-      <c r="CM30" s="22"/>
-      <c r="CN30" s="22"/>
-      <c r="CO30" s="22"/>
+      <c r="BM30" s="21"/>
+      <c r="BN30" s="21"/>
+      <c r="BO30" s="21"/>
+      <c r="BP30" s="21"/>
+      <c r="BQ30" s="21"/>
+      <c r="BR30" s="21"/>
+      <c r="BS30" s="21"/>
+      <c r="BT30" s="21"/>
+      <c r="BU30" s="21"/>
+      <c r="BV30" s="21"/>
+      <c r="BW30" s="21"/>
+      <c r="BX30" s="21"/>
+      <c r="BY30" s="21"/>
+      <c r="BZ30" s="21"/>
+      <c r="CA30" s="21"/>
+      <c r="CB30" s="21"/>
+      <c r="CC30" s="21"/>
+      <c r="CD30" s="21"/>
+      <c r="CE30" s="21"/>
+      <c r="CF30" s="21"/>
+      <c r="CG30" s="21"/>
+      <c r="CH30" s="21"/>
+      <c r="CI30" s="21"/>
+      <c r="CJ30" s="21"/>
+      <c r="CK30" s="21"/>
+      <c r="CL30" s="21"/>
+      <c r="CM30" s="21"/>
+      <c r="CN30" s="21"/>
+      <c r="CO30" s="21"/>
     </row>
     <row r="31" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
-      <c r="BM31" s="22"/>
-      <c r="BN31" s="22"/>
-      <c r="BO31" s="22"/>
-      <c r="BP31" s="22"/>
-      <c r="BQ31" s="22"/>
-      <c r="BR31" s="22"/>
-      <c r="BS31" s="22"/>
-      <c r="BT31" s="22"/>
-      <c r="BU31" s="22"/>
-      <c r="BV31" s="22"/>
-      <c r="BW31" s="22"/>
-      <c r="BX31" s="22"/>
-      <c r="BY31" s="22"/>
-      <c r="BZ31" s="22"/>
-      <c r="CA31" s="22"/>
-      <c r="CB31" s="22"/>
-      <c r="CC31" s="22"/>
-      <c r="CD31" s="22"/>
-      <c r="CE31" s="22"/>
-      <c r="CF31" s="22"/>
-      <c r="CG31" s="22"/>
-      <c r="CH31" s="22"/>
-      <c r="CI31" s="22"/>
-      <c r="CJ31" s="22"/>
-      <c r="CK31" s="22"/>
-      <c r="CL31" s="22"/>
-      <c r="CM31" s="22"/>
-      <c r="CN31" s="22"/>
-      <c r="CO31" s="22"/>
+      <c r="M31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="V31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="W31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="X31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="BM31" s="21"/>
+      <c r="BN31" s="21"/>
+      <c r="BO31" s="21"/>
+      <c r="BP31" s="21"/>
+      <c r="BQ31" s="21"/>
+      <c r="BR31" s="21"/>
+      <c r="BS31" s="21"/>
+      <c r="BT31" s="21"/>
+      <c r="BU31" s="21"/>
+      <c r="BV31" s="21"/>
+      <c r="BW31" s="21"/>
+      <c r="BX31" s="21"/>
+      <c r="BY31" s="21"/>
+      <c r="BZ31" s="21"/>
+      <c r="CA31" s="21"/>
+      <c r="CB31" s="21"/>
+      <c r="CC31" s="21"/>
+      <c r="CD31" s="21"/>
+      <c r="CE31" s="21"/>
+      <c r="CF31" s="21"/>
+      <c r="CG31" s="21"/>
+      <c r="CH31" s="21"/>
+      <c r="CI31" s="21"/>
+      <c r="CJ31" s="21"/>
+      <c r="CK31" s="21"/>
+      <c r="CL31" s="21"/>
+      <c r="CM31" s="21"/>
+      <c r="CN31" s="21"/>
+      <c r="CO31" s="21"/>
     </row>
     <row r="32" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
-      <c r="BM32" s="22"/>
-      <c r="BN32" s="22"/>
-      <c r="BO32" s="22"/>
-      <c r="BP32" s="22"/>
-      <c r="BQ32" s="22"/>
-      <c r="BR32" s="22"/>
-      <c r="BS32" s="22"/>
-      <c r="BT32" s="22"/>
-      <c r="BU32" s="22"/>
-      <c r="BV32" s="22"/>
-      <c r="BW32" s="22"/>
-      <c r="BX32" s="22"/>
-      <c r="BY32" s="22"/>
-      <c r="BZ32" s="22"/>
-      <c r="CA32" s="22"/>
-      <c r="CB32" s="22"/>
-      <c r="CC32" s="22"/>
-      <c r="CD32" s="22"/>
-      <c r="CE32" s="22"/>
-      <c r="CF32" s="22"/>
-      <c r="CG32" s="22"/>
-      <c r="CH32" s="22"/>
-      <c r="CI32" s="22"/>
-      <c r="CJ32" s="22"/>
-      <c r="CK32" s="22"/>
-      <c r="CL32" s="22"/>
-      <c r="CM32" s="22"/>
-      <c r="CN32" s="22"/>
-      <c r="CO32" s="22"/>
+      <c r="BM32" s="21"/>
+      <c r="BN32" s="21"/>
+      <c r="BO32" s="21"/>
+      <c r="BP32" s="21"/>
+      <c r="BQ32" s="21"/>
+      <c r="BR32" s="21"/>
+      <c r="BS32" s="21"/>
+      <c r="BT32" s="21"/>
+      <c r="BU32" s="21"/>
+      <c r="BV32" s="21"/>
+      <c r="BW32" s="21"/>
+      <c r="BX32" s="21"/>
+      <c r="BY32" s="21"/>
+      <c r="BZ32" s="21"/>
+      <c r="CA32" s="21"/>
+      <c r="CB32" s="21"/>
+      <c r="CC32" s="21"/>
+      <c r="CD32" s="21"/>
+      <c r="CE32" s="21"/>
+      <c r="CF32" s="21"/>
+      <c r="CG32" s="21"/>
+      <c r="CH32" s="21"/>
+      <c r="CI32" s="21"/>
+      <c r="CJ32" s="21"/>
+      <c r="CK32" s="21"/>
+      <c r="CL32" s="21"/>
+      <c r="CM32" s="21"/>
+      <c r="CN32" s="21"/>
+      <c r="CO32" s="21"/>
     </row>
     <row r="33" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
@@ -3284,88 +3332,78 @@
         <v>3</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N33" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O33" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="P33" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I33" s="4" t="s">
+      <c r="Q33" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J33" s="4" t="s">
+      <c r="R33" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="S33" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K33" s="4" t="s">
+      <c r="T33" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="L33" s="4" t="s">
+      <c r="U33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="V33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="W33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="X33" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="M33" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="N33" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="O33" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="P33" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q33" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="R33" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="S33" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="T33" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="U33" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="V33" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="W33" s="4" t="s">
+      <c r="Y33" s="4"/>
+      <c r="Z33" s="4"/>
+      <c r="AA33" s="4"/>
+      <c r="AB33" s="4"/>
+      <c r="AC33" s="4"/>
+      <c r="AD33" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="X33" s="4" t="s">
+      <c r="AE33" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="Y33" s="4" t="s">
+      <c r="AF33" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="Z33" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA33" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB33" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC33" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD33" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AE33" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF33" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="AG33" s="4" t="s">
         <v>3</v>
@@ -3374,62 +3412,42 @@
         <v>3</v>
       </c>
       <c r="AI33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AL33" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AM33" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AN33" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AO33" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="AJ33" s="4" t="s">
+      <c r="AP33" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="AK33" s="4" t="s">
+      <c r="AQ33" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="AL33" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AM33" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AN33" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AO33" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AP33" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AQ33" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AR33" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AS33" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AT33" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AU33" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AV33" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AW33" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AX33" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AY33" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="AZ33" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="BA33" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="AR33" s="4"/>
+      <c r="AS33" s="4"/>
+      <c r="AT33" s="4"/>
+      <c r="AU33" s="4"/>
+      <c r="AV33" s="4"/>
+      <c r="AW33" s="4"/>
+      <c r="AX33" s="4"/>
+      <c r="AY33" s="4"/>
+      <c r="AZ33" s="4"/>
+      <c r="BA33" s="4"/>
       <c r="BB33" s="4"/>
     </row>
     <row r="34" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3439,32 +3457,24 @@
       <c r="B34" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F34" s="13" t="s">
+      <c r="D34" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M34" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="V34" s="1" t="s">
+      <c r="F34" s="13"/>
+      <c r="I34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O34" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AC34" s="1" t="s">
+      <c r="T34" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="X34" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="AH34" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AO34" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="AT34" t="s">
-        <v>29</v>
-      </c>
-      <c r="AV34" t="s">
-        <v>15</v>
-      </c>
-      <c r="AX34" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3502,16 +3512,34 @@
       <c r="U36" s="4"/>
       <c r="V36" s="4"/>
       <c r="W36" s="4"/>
-      <c r="X36" s="4"/>
-      <c r="Y36" s="4"/>
-      <c r="Z36" s="4"/>
-      <c r="AA36" s="4"/>
-      <c r="AB36" s="4"/>
-      <c r="AC36" s="4"/>
-      <c r="AD36" s="4"/>
-      <c r="AE36" s="4"/>
-      <c r="AF36" s="4"/>
-      <c r="AG36" s="5" t="s">
+      <c r="X36" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG36" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AH36" s="4" t="s">
@@ -3526,41 +3554,74 @@
       <c r="AK36" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AL36" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AM36" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AN36" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AO36" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AP36" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AQ36" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AR36" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AS36" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AT36" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AU36" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="AV36" s="3" t="s">
+      <c r="AL36" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM36" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="AN36" s="4"/>
+      <c r="AO36" s="4"/>
+      <c r="AP36" s="4"/>
+      <c r="AQ36" s="4"/>
+      <c r="AR36" s="4"/>
+      <c r="AS36" s="4"/>
+      <c r="AT36" s="4"/>
+      <c r="AU36" s="4"/>
+      <c r="AV36" s="4"/>
       <c r="AW36" s="4"/>
       <c r="AX36" s="4"/>
+      <c r="AY36" s="4"/>
+      <c r="AZ36" s="4"/>
+      <c r="BA36" s="4"/>
+      <c r="BB36" s="4"/>
+    </row>
+    <row r="37" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="X37" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z37" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB37" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD37" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF37" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH37" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AJ37" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AK37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL37" s="13" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="41" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="42" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4409,14 +4470,14 @@
     </row>
     <row r="69" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="3"/>
-      <c r="AU69" s="22"/>
-      <c r="AV69" s="22"/>
-      <c r="AW69" s="22"/>
-      <c r="AX69" s="22"/>
-      <c r="AY69" s="22"/>
-      <c r="AZ69" s="22"/>
-      <c r="BA69" s="22"/>
-      <c r="BB69" s="22"/>
+      <c r="AU69" s="21"/>
+      <c r="AV69" s="21"/>
+      <c r="AW69" s="21"/>
+      <c r="AX69" s="21"/>
+      <c r="AY69" s="21"/>
+      <c r="AZ69" s="21"/>
+      <c r="BA69" s="21"/>
+      <c r="BB69" s="21"/>
     </row>
     <row r="70" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">

</xml_diff>

<commit_message>
III-3 début sec 1 rapport et début sec 2 + début rdpt
</commit_message>
<xml_diff>
--- a/ordo.xlsx
+++ b/ordo.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9648" tabRatio="289"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9648" tabRatio="171" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="37">
   <si>
     <t>P1</t>
   </si>
@@ -126,6 +127,15 @@
   </si>
   <si>
     <t>Chariot</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Charriot</t>
+  </si>
+  <si>
+    <t>Position</t>
   </si>
 </sst>
 </file>
@@ -793,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CX74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AL37" sqref="AL37"/>
+    <sheetView zoomScale="43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:CX18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1430,8 +1440,10 @@
       <c r="AQ11" s="24"/>
       <c r="AR11" s="24"/>
       <c r="AS11" s="24"/>
-      <c r="AT11" s="24"/>
-      <c r="AU11" s="23" t="s">
+      <c r="AT11" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="AU11" s="24" t="s">
         <v>23</v>
       </c>
       <c r="AV11" s="24" t="s">
@@ -1503,12 +1515,10 @@
       <c r="BR11" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="BS11" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="BT11" s="25" t="s">
-        <v>23</v>
-      </c>
+      <c r="BS11" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="BT11" s="24"/>
       <c r="BU11" s="24"/>
       <c r="BV11" s="24"/>
       <c r="BW11" s="24"/>
@@ -1649,6 +1659,9 @@
       <c r="AO12" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="AT12" t="s">
+        <v>31</v>
+      </c>
       <c r="AU12" t="s">
         <v>31</v>
       </c>
@@ -1726,6 +1739,66 @@
       </c>
       <c r="BT12" t="s">
         <v>31</v>
+      </c>
+      <c r="BZ12" t="s">
+        <v>32</v>
+      </c>
+      <c r="CA12" t="s">
+        <v>32</v>
+      </c>
+      <c r="CB12" t="s">
+        <v>32</v>
+      </c>
+      <c r="CC12" t="s">
+        <v>32</v>
+      </c>
+      <c r="CD12" t="s">
+        <v>32</v>
+      </c>
+      <c r="CE12" t="s">
+        <v>32</v>
+      </c>
+      <c r="CF12" t="s">
+        <v>32</v>
+      </c>
+      <c r="CG12" t="s">
+        <v>32</v>
+      </c>
+      <c r="CH12" t="s">
+        <v>32</v>
+      </c>
+      <c r="CI12" t="s">
+        <v>32</v>
+      </c>
+      <c r="CJ12" t="s">
+        <v>32</v>
+      </c>
+      <c r="CK12" t="s">
+        <v>32</v>
+      </c>
+      <c r="CL12" t="s">
+        <v>32</v>
+      </c>
+      <c r="CM12" t="s">
+        <v>32</v>
+      </c>
+      <c r="CN12" t="s">
+        <v>32</v>
+      </c>
+      <c r="CO12" t="s">
+        <v>32</v>
+      </c>
+      <c r="CP12" t="s">
+        <v>32</v>
+      </c>
+      <c r="CQ12" t="s">
+        <v>32</v>
+      </c>
+      <c r="CR12" t="s">
+        <v>32</v>
+      </c>
+      <c r="CS12" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1812,7 +1885,7 @@
         <v>3</v>
       </c>
       <c r="AD14" s="37" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="AE14" s="37" t="s">
         <v>8</v>
@@ -1821,15 +1894,15 @@
         <v>8</v>
       </c>
       <c r="AG14" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="AH14" s="37" t="s">
         <v>13</v>
       </c>
+      <c r="AH14" s="37"/>
       <c r="AI14" s="37"/>
       <c r="AJ14" s="37"/>
       <c r="AK14" s="37"/>
-      <c r="AL14" s="37"/>
+      <c r="AL14" s="37" t="s">
+        <v>9</v>
+      </c>
       <c r="AM14" s="37" t="s">
         <v>9</v>
       </c>
@@ -1837,13 +1910,13 @@
         <v>9</v>
       </c>
       <c r="AO14" s="37" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="AP14" s="37" t="s">
         <v>3</v>
       </c>
       <c r="AQ14" s="37" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="AR14" s="37" t="s">
         <v>8</v>
@@ -1851,15 +1924,15 @@
       <c r="AS14" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="AT14" s="37" t="s">
-        <v>8</v>
-      </c>
+      <c r="AT14" s="37"/>
       <c r="AU14" s="37"/>
       <c r="AV14" s="37"/>
       <c r="AW14" s="37"/>
-      <c r="AX14" s="37"/>
+      <c r="AX14" s="37" t="s">
+        <v>13</v>
+      </c>
       <c r="AY14" s="37" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="AZ14" s="37" t="s">
         <v>9</v>
@@ -1868,33 +1941,35 @@
         <v>9</v>
       </c>
       <c r="BB14" s="37" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="BC14" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="BD14" s="37" t="s">
-        <v>3</v>
-      </c>
+      <c r="BD14" s="37"/>
       <c r="BE14" s="37"/>
       <c r="BF14" s="37"/>
       <c r="BG14" s="37"/>
       <c r="BH14" s="37"/>
       <c r="BI14" s="37"/>
-      <c r="BJ14" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="BK14" s="37" t="s">
-        <v>8</v>
-      </c>
+      <c r="BJ14" s="37"/>
+      <c r="BK14" s="37"/>
       <c r="BL14" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="BM14" s="37"/>
-      <c r="BN14" s="37"/>
-      <c r="BO14" s="37"/>
+      <c r="BM14" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="BN14" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="BO14" s="37" t="s">
+        <v>13</v>
+      </c>
       <c r="BP14" s="37"/>
-      <c r="BQ14" s="37"/>
+      <c r="BQ14" s="37" t="s">
+        <v>9</v>
+      </c>
       <c r="BR14" s="37" t="s">
         <v>9</v>
       </c>
@@ -1902,13 +1977,13 @@
         <v>9</v>
       </c>
       <c r="BT14" s="37" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="BU14" s="37" t="s">
         <v>3</v>
       </c>
       <c r="BV14" s="37" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="BW14" s="37" t="s">
         <v>8</v>
@@ -1967,34 +2042,38 @@
       <c r="U15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="AD15" s="20" t="s">
+      <c r="AC15" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="AE15" s="20"/>
-      <c r="AH15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AQ15" t="s">
+      <c r="AD15" s="20"/>
+      <c r="AG15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AO15"/>
+      <c r="AP15" t="s">
         <v>31</v>
       </c>
-      <c r="AY15" t="s">
+      <c r="AX15" t="s">
         <v>29</v>
       </c>
-      <c r="BD15" t="s">
+      <c r="BC15" t="s">
         <v>30</v>
       </c>
+      <c r="BL15" s="21"/>
       <c r="BM15" s="21"/>
       <c r="BN15" s="21"/>
-      <c r="BO15" s="21"/>
+      <c r="BO15" s="21" t="s">
+        <v>31</v>
+      </c>
       <c r="BP15" s="21"/>
       <c r="BQ15" s="21"/>
       <c r="BR15" s="21"/>
       <c r="BS15" s="21"/>
       <c r="BT15" s="21"/>
-      <c r="BU15" s="21"/>
-      <c r="BV15" s="21" t="s">
+      <c r="BU15" s="21" t="s">
         <v>32</v>
       </c>
+      <c r="BV15" s="21"/>
       <c r="BW15" s="21"/>
       <c r="BX15" s="21"/>
       <c r="BY15" s="21"/>
@@ -2114,8 +2193,10 @@
       <c r="AD17" s="29"/>
       <c r="AE17" s="29"/>
       <c r="AF17" s="29"/>
-      <c r="AG17" s="29"/>
-      <c r="AH17" s="28" t="s">
+      <c r="AG17" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH17" s="29" t="s">
         <v>22</v>
       </c>
       <c r="AI17" s="29" t="s">
@@ -2169,18 +2250,16 @@
       <c r="AY17" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="AZ17" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="BA17" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="BB17" s="28" t="s">
+      <c r="AZ17" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="BA17" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="BC17" s="30" t="s">
+      <c r="BB17" s="30" t="s">
         <v>12</v>
       </c>
+      <c r="BC17" s="29"/>
       <c r="BD17" s="29"/>
       <c r="BE17" s="29"/>
       <c r="BF17" s="29"/>
@@ -2191,10 +2270,8 @@
       <c r="BK17" s="29"/>
       <c r="BL17" s="29"/>
       <c r="BM17" s="29"/>
-      <c r="BN17" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="BO17" s="29" t="s">
+      <c r="BN17" s="29"/>
+      <c r="BO17" s="28" t="s">
         <v>24</v>
       </c>
       <c r="BP17" s="29" t="s">
@@ -2236,13 +2313,15 @@
       <c r="CB17" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="CC17" s="30" t="s">
+      <c r="CC17" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="CD17" s="27" t="s">
+      <c r="CD17" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="CE17" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="CE17" s="29"/>
       <c r="CF17" s="29"/>
       <c r="CG17" s="29"/>
       <c r="CH17" s="29"/>
@@ -2309,69 +2388,65 @@
       <c r="Z18" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="AH18" s="13" t="s">
+      <c r="AG18" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AI18" s="1" t="s">
+      <c r="AH18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AJ18" s="13" t="s">
+      <c r="AI18" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AK18" s="1" t="s">
+      <c r="AJ18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AL18" s="13" t="s">
+      <c r="AK18" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AM18" s="1" t="s">
+      <c r="AL18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AN18" s="13" t="s">
+      <c r="AM18" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AO18" s="1" t="s">
+      <c r="AN18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AP18" s="13" t="s">
+      <c r="AO18" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AQ18" s="1" t="s">
+      <c r="AP18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AR18" s="13" t="s">
+      <c r="AQ18" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AS18" s="1" t="s">
+      <c r="AR18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AT18" s="13" t="s">
+      <c r="AS18" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AU18" s="1" t="s">
+      <c r="AT18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AV18" s="13" t="s">
+      <c r="AU18" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AW18" s="1" t="s">
+      <c r="AV18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AX18" s="13" t="s">
+      <c r="AW18" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AY18" s="1" t="s">
+      <c r="AX18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AZ18" s="13" t="s">
+      <c r="AY18" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="BA18" s="1" t="s">
+      <c r="AZ18" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="BM18" s="21"/>
-      <c r="BN18" s="21" t="s">
-        <v>30</v>
       </c>
       <c r="BO18" s="21" t="s">
         <v>30</v>
@@ -2418,7 +2493,9 @@
       <c r="CC18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="CD18" s="21"/>
+      <c r="CD18" s="21" t="s">
+        <v>30</v>
+      </c>
       <c r="CE18" s="21"/>
       <c r="CF18" s="21"/>
       <c r="CG18" s="21"/>
@@ -2432,6 +2509,9 @@
       <c r="CO18" s="21"/>
     </row>
     <row r="19" spans="1:102" x14ac:dyDescent="0.3">
+      <c r="BI19" t="s">
+        <v>34</v>
+      </c>
       <c r="BZ19" s="21"/>
       <c r="CA19" s="21"/>
       <c r="CB19" s="21"/>
@@ -4547,4 +4627,2145 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="22" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AZ28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.77734375" customWidth="1"/>
+    <col min="2" max="41" width="3.6640625" customWidth="1"/>
+    <col min="42" max="50" width="3.5546875"/>
+    <col min="51" max="51" width="4.44140625" customWidth="1"/>
+    <col min="52" max="101" width="3.5546875"/>
+    <col min="102" max="102" width="4.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="1"/>
+      <c r="AM1" s="1"/>
+      <c r="AN1" s="1"/>
+      <c r="AO1" s="1"/>
+    </row>
+    <row r="2" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="39"/>
+      <c r="N2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="39"/>
+      <c r="P2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="1"/>
+      <c r="AM2" s="1"/>
+      <c r="AN2" s="1"/>
+      <c r="AO2" s="1"/>
+    </row>
+    <row r="3" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9">
+        <v>2</v>
+      </c>
+      <c r="D3" s="9">
+        <v>3</v>
+      </c>
+      <c r="E3" s="9">
+        <v>4</v>
+      </c>
+      <c r="F3" s="9">
+        <v>5</v>
+      </c>
+      <c r="G3" s="10">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="43"/>
+      <c r="N3" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="43"/>
+      <c r="P3" s="44"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="1"/>
+      <c r="AJ3" s="1"/>
+      <c r="AK3" s="1"/>
+      <c r="AL3" s="1"/>
+      <c r="AM3" s="1"/>
+      <c r="AN3" s="1"/>
+      <c r="AO3" s="1"/>
+      <c r="AP3" s="1"/>
+    </row>
+    <row r="4" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="7">
+        <v>15</v>
+      </c>
+      <c r="C4" s="7">
+        <v>20</v>
+      </c>
+      <c r="D4" s="7">
+        <v>20</v>
+      </c>
+      <c r="E4" s="7">
+        <v>26</v>
+      </c>
+      <c r="F4" s="7">
+        <v>16</v>
+      </c>
+      <c r="G4" s="12">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
+      <c r="AG4" s="1"/>
+      <c r="AH4" s="1"/>
+      <c r="AI4" s="1"/>
+      <c r="AJ4" s="1"/>
+      <c r="AK4" s="1"/>
+      <c r="AL4" s="1"/>
+      <c r="AM4" s="1"/>
+      <c r="AN4" s="1"/>
+      <c r="AO4" s="1"/>
+      <c r="AP4" s="1"/>
+    </row>
+    <row r="5" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="15">
+        <v>16</v>
+      </c>
+      <c r="C5" s="15">
+        <v>22</v>
+      </c>
+      <c r="D5" s="15">
+        <v>22</v>
+      </c>
+      <c r="E5" s="15">
+        <v>28</v>
+      </c>
+      <c r="F5" s="15">
+        <v>17</v>
+      </c>
+      <c r="G5" s="16">
+        <v>22</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="39"/>
+      <c r="N5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="39"/>
+      <c r="P5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1"/>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1"/>
+      <c r="AI5" s="1"/>
+      <c r="AJ5" s="1"/>
+      <c r="AK5" s="1"/>
+      <c r="AL5" s="1"/>
+      <c r="AM5" s="1"/>
+      <c r="AN5" s="1"/>
+      <c r="AO5" s="1"/>
+      <c r="AP5" s="1"/>
+    </row>
+    <row r="6" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="7">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7">
+        <v>2</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="43"/>
+      <c r="N6" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="O6" s="43"/>
+      <c r="P6" s="44"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1"/>
+      <c r="AG6" s="1"/>
+      <c r="AH6" s="1"/>
+      <c r="AI6" s="1"/>
+      <c r="AJ6" s="1"/>
+      <c r="AK6" s="1"/>
+      <c r="AL6" s="1"/>
+      <c r="AM6" s="1"/>
+      <c r="AN6" s="1"/>
+      <c r="AO6" s="1"/>
+      <c r="AP6" s="1"/>
+    </row>
+    <row r="7" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="39"/>
+      <c r="O7" s="39"/>
+      <c r="P7" s="39"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="1"/>
+      <c r="AG7" s="1"/>
+      <c r="AH7" s="1"/>
+      <c r="AI7" s="1"/>
+      <c r="AJ7" s="1"/>
+      <c r="AK7" s="1"/>
+      <c r="AL7" s="1"/>
+      <c r="AM7" s="1"/>
+      <c r="AN7" s="1"/>
+      <c r="AO7" s="1"/>
+      <c r="AP7" s="1"/>
+    </row>
+    <row r="8" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="40">
+        <v>0</v>
+      </c>
+      <c r="C8" s="33">
+        <v>1</v>
+      </c>
+      <c r="D8" s="33">
+        <v>2</v>
+      </c>
+      <c r="E8" s="33">
+        <v>3</v>
+      </c>
+      <c r="F8" s="33">
+        <v>4</v>
+      </c>
+      <c r="G8" s="33">
+        <v>5</v>
+      </c>
+      <c r="H8" s="33">
+        <v>6</v>
+      </c>
+      <c r="I8" s="33">
+        <v>7</v>
+      </c>
+      <c r="J8" s="33">
+        <v>8</v>
+      </c>
+      <c r="K8" s="33">
+        <v>9</v>
+      </c>
+      <c r="L8" s="33">
+        <v>10</v>
+      </c>
+      <c r="M8" s="33">
+        <v>11</v>
+      </c>
+      <c r="N8" s="33">
+        <v>12</v>
+      </c>
+      <c r="O8" s="33">
+        <v>13</v>
+      </c>
+      <c r="P8" s="33">
+        <v>14</v>
+      </c>
+      <c r="Q8" s="33">
+        <v>15</v>
+      </c>
+      <c r="R8" s="33">
+        <v>16</v>
+      </c>
+      <c r="S8" s="33">
+        <v>17</v>
+      </c>
+      <c r="T8" s="33">
+        <v>18</v>
+      </c>
+      <c r="U8" s="33">
+        <v>19</v>
+      </c>
+      <c r="V8" s="33">
+        <v>20</v>
+      </c>
+      <c r="W8" s="33">
+        <v>21</v>
+      </c>
+      <c r="X8" s="33">
+        <v>22</v>
+      </c>
+      <c r="Y8" s="33">
+        <v>23</v>
+      </c>
+      <c r="Z8" s="33">
+        <v>24</v>
+      </c>
+      <c r="AA8" s="33">
+        <v>25</v>
+      </c>
+      <c r="AB8" s="33">
+        <v>26</v>
+      </c>
+      <c r="AC8" s="33">
+        <v>27</v>
+      </c>
+      <c r="AD8" s="33">
+        <v>28</v>
+      </c>
+      <c r="AE8" s="33">
+        <v>29</v>
+      </c>
+      <c r="AF8" s="33">
+        <v>30</v>
+      </c>
+      <c r="AG8" s="33">
+        <v>31</v>
+      </c>
+      <c r="AH8" s="33">
+        <v>32</v>
+      </c>
+      <c r="AI8" s="33">
+        <v>33</v>
+      </c>
+      <c r="AJ8" s="33">
+        <v>34</v>
+      </c>
+      <c r="AK8" s="33">
+        <v>35</v>
+      </c>
+      <c r="AL8" s="33">
+        <v>36</v>
+      </c>
+      <c r="AM8" s="33">
+        <v>37</v>
+      </c>
+      <c r="AN8" s="33">
+        <v>38</v>
+      </c>
+      <c r="AO8" s="33">
+        <v>39</v>
+      </c>
+      <c r="AP8" s="33">
+        <v>40</v>
+      </c>
+      <c r="AQ8" s="33">
+        <v>41</v>
+      </c>
+      <c r="AR8" s="33">
+        <v>42</v>
+      </c>
+      <c r="AS8" s="33">
+        <v>43</v>
+      </c>
+      <c r="AT8" s="33">
+        <v>44</v>
+      </c>
+      <c r="AU8" s="33">
+        <v>45</v>
+      </c>
+      <c r="AV8" s="33">
+        <v>46</v>
+      </c>
+      <c r="AW8" s="33">
+        <v>47</v>
+      </c>
+      <c r="AX8" s="33">
+        <v>48</v>
+      </c>
+      <c r="AY8" s="33">
+        <v>49</v>
+      </c>
+      <c r="AZ8" s="33">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="1"/>
+      <c r="AF9" s="1"/>
+      <c r="AG9" s="1"/>
+      <c r="AH9" s="1"/>
+      <c r="AI9" s="1"/>
+      <c r="AJ9" s="1"/>
+      <c r="AK9" s="1"/>
+      <c r="AL9" s="1"/>
+      <c r="AM9" s="1"/>
+      <c r="AN9" s="1"/>
+      <c r="AO9" s="1"/>
+    </row>
+    <row r="10" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="23"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="24"/>
+      <c r="T10" s="24"/>
+      <c r="U10" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="V10" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="W10" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="X10" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y10" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z10" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA10" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB10" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC10" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD10" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE10" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF10" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG10" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH10" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI10" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AJ10" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AK10" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AL10" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AM10" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AN10" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="AO10" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP10" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ10" s="24"/>
+      <c r="AR10" s="24"/>
+      <c r="AS10" s="24"/>
+      <c r="AT10" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="AU10" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="AV10" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="AW10" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="AX10" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="AY10" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="AZ10" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="3"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AN11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AO11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AT11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AU11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AV11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AW11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AX11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AY11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AZ11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="3"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="1"/>
+      <c r="AE12" s="1"/>
+      <c r="AF12" s="1"/>
+      <c r="AG12" s="1"/>
+      <c r="AH12" s="1"/>
+      <c r="AI12" s="1"/>
+      <c r="AJ12" s="1"/>
+      <c r="AK12" s="1"/>
+      <c r="AL12" s="1"/>
+      <c r="AM12" s="1"/>
+      <c r="AN12" s="1"/>
+      <c r="AO12" s="1"/>
+    </row>
+    <row r="13" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="36"/>
+      <c r="C13" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="J13" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="K13" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="L13" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="M13" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="N13" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="O13" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="P13" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q13" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="R13" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="S13" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="T13" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="U13" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="V13" s="37"/>
+      <c r="W13" s="37"/>
+      <c r="X13" s="37"/>
+      <c r="Y13" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z13" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA13" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB13" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC13" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD13" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE13" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF13" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG13" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH13" s="37"/>
+      <c r="AI13" s="37"/>
+      <c r="AJ13" s="37"/>
+      <c r="AK13" s="37"/>
+      <c r="AL13" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="AM13" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="AN13" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="AO13" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="AP13" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ13" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR13" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="AS13" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT13" s="37"/>
+      <c r="AU13" s="37"/>
+      <c r="AV13" s="37"/>
+      <c r="AW13" s="37"/>
+      <c r="AX13" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="AY13" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="AZ13" s="37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD14" s="20"/>
+      <c r="AE14" s="1"/>
+      <c r="AF14" s="1"/>
+      <c r="AG14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH14" s="1"/>
+      <c r="AI14" s="1"/>
+      <c r="AJ14" s="1"/>
+      <c r="AK14" s="1"/>
+      <c r="AL14" s="1"/>
+      <c r="AM14" s="1"/>
+      <c r="AN14" s="1"/>
+      <c r="AP14" t="s">
+        <v>31</v>
+      </c>
+      <c r="AX14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="3"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+      <c r="AD15" s="1"/>
+      <c r="AE15" s="1"/>
+      <c r="AF15" s="1"/>
+      <c r="AG15" s="1"/>
+      <c r="AH15" s="1"/>
+      <c r="AI15" s="1"/>
+      <c r="AJ15" s="1"/>
+      <c r="AK15" s="1"/>
+      <c r="AL15" s="1"/>
+      <c r="AM15" s="1"/>
+      <c r="AN15" s="1"/>
+      <c r="AO15" s="1"/>
+    </row>
+    <row r="16" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="28"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="M16" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="N16" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="O16" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="P16" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q16" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="R16" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="S16" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="T16" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="U16" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="V16" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="W16" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="X16" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y16" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z16" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA16" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB16" s="29"/>
+      <c r="AC16" s="29"/>
+      <c r="AD16" s="29"/>
+      <c r="AE16" s="29"/>
+      <c r="AF16" s="29"/>
+      <c r="AG16" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH16" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AI16" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ16" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK16" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AL16" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM16" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AN16" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO16" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AP16" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AQ16" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AR16" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AS16" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AT16" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU16" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV16" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AW16" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AX16" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY16" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ16" s="30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N17" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P17" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R17" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="T17" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V17" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="W17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="X17" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z17" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1"/>
+      <c r="AD17" s="1"/>
+      <c r="AE17" s="1"/>
+      <c r="AF17" s="1"/>
+      <c r="AG17" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI17" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK17" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM17" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="AN17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO17" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="AP17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AQ17" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="AR17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AS17" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="AT17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AU17" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="AV17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AW17" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="AX17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AY17" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="AZ17" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="33">
+        <v>51</v>
+      </c>
+      <c r="C19" s="33">
+        <v>52</v>
+      </c>
+      <c r="D19" s="33">
+        <v>53</v>
+      </c>
+      <c r="E19" s="33">
+        <v>54</v>
+      </c>
+      <c r="F19" s="33">
+        <v>55</v>
+      </c>
+      <c r="G19" s="33">
+        <v>56</v>
+      </c>
+      <c r="H19" s="33">
+        <v>57</v>
+      </c>
+      <c r="I19" s="33">
+        <v>58</v>
+      </c>
+      <c r="J19" s="33">
+        <v>59</v>
+      </c>
+      <c r="K19" s="33">
+        <v>60</v>
+      </c>
+      <c r="L19" s="33">
+        <v>61</v>
+      </c>
+      <c r="M19" s="33">
+        <v>62</v>
+      </c>
+      <c r="N19" s="33">
+        <v>63</v>
+      </c>
+      <c r="O19" s="33">
+        <v>64</v>
+      </c>
+      <c r="P19" s="33">
+        <v>65</v>
+      </c>
+      <c r="Q19" s="33">
+        <v>66</v>
+      </c>
+      <c r="R19" s="33">
+        <v>67</v>
+      </c>
+      <c r="S19" s="33">
+        <v>68</v>
+      </c>
+      <c r="T19" s="33">
+        <v>69</v>
+      </c>
+      <c r="U19" s="33">
+        <v>70</v>
+      </c>
+      <c r="V19" s="33">
+        <v>71</v>
+      </c>
+      <c r="W19" s="33">
+        <v>72</v>
+      </c>
+      <c r="X19" s="33">
+        <v>73</v>
+      </c>
+      <c r="Y19" s="33">
+        <v>74</v>
+      </c>
+      <c r="Z19" s="33">
+        <v>75</v>
+      </c>
+      <c r="AA19" s="33">
+        <v>76</v>
+      </c>
+      <c r="AB19" s="33">
+        <v>77</v>
+      </c>
+      <c r="AC19" s="33">
+        <v>78</v>
+      </c>
+      <c r="AD19" s="33">
+        <v>79</v>
+      </c>
+      <c r="AE19" s="33">
+        <v>80</v>
+      </c>
+      <c r="AF19" s="33">
+        <v>81</v>
+      </c>
+      <c r="AG19" s="33">
+        <v>82</v>
+      </c>
+      <c r="AH19" s="33">
+        <v>83</v>
+      </c>
+      <c r="AI19" s="33">
+        <v>84</v>
+      </c>
+      <c r="AJ19" s="33">
+        <v>85</v>
+      </c>
+      <c r="AK19" s="33">
+        <v>86</v>
+      </c>
+      <c r="AL19" s="33">
+        <v>87</v>
+      </c>
+      <c r="AM19" s="33">
+        <v>88</v>
+      </c>
+      <c r="AN19" s="33">
+        <v>89</v>
+      </c>
+      <c r="AO19" s="33">
+        <v>90</v>
+      </c>
+      <c r="AP19" s="33">
+        <v>91</v>
+      </c>
+      <c r="AQ19" s="33">
+        <v>92</v>
+      </c>
+      <c r="AR19" s="33">
+        <v>93</v>
+      </c>
+      <c r="AS19" s="33">
+        <v>94</v>
+      </c>
+      <c r="AT19" s="33">
+        <v>95</v>
+      </c>
+      <c r="AU19" s="33">
+        <v>96</v>
+      </c>
+      <c r="AV19" s="33">
+        <v>97</v>
+      </c>
+      <c r="AW19" s="33">
+        <v>98</v>
+      </c>
+      <c r="AX19" s="33">
+        <v>99</v>
+      </c>
+      <c r="AY19" s="33">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="J21" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="L21" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="M21" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="N21" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="O21" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="P21" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q21" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="R21" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="S21" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="T21" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="U21" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="V21" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="W21" s="24"/>
+      <c r="X21" s="24"/>
+      <c r="Y21" s="24"/>
+      <c r="Z21" s="24"/>
+      <c r="AA21" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB21" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC21" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD21" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE21" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF21" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG21" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH21" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI21" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="AJ21" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="AK21" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="AL21" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="AM21" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="AN21" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="AO21" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="AP21" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="AQ21" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="AR21" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="AS21" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="AT21" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="AU21" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="AV21" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW21" s="24"/>
+      <c r="AX21" s="24"/>
+      <c r="AY21" s="24"/>
+      <c r="AZ21" s="24"/>
+    </row>
+    <row r="22" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="3"/>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" t="s">
+        <v>31</v>
+      </c>
+      <c r="H22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" t="s">
+        <v>31</v>
+      </c>
+      <c r="J22" t="s">
+        <v>31</v>
+      </c>
+      <c r="K22" t="s">
+        <v>31</v>
+      </c>
+      <c r="L22" t="s">
+        <v>31</v>
+      </c>
+      <c r="M22" t="s">
+        <v>31</v>
+      </c>
+      <c r="N22" t="s">
+        <v>31</v>
+      </c>
+      <c r="O22" t="s">
+        <v>31</v>
+      </c>
+      <c r="P22" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>31</v>
+      </c>
+      <c r="R22" t="s">
+        <v>31</v>
+      </c>
+      <c r="S22" t="s">
+        <v>31</v>
+      </c>
+      <c r="T22" t="s">
+        <v>31</v>
+      </c>
+      <c r="U22" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AO22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AQ22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AR22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AS22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="3"/>
+    </row>
+    <row r="24" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="37"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="N24" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="O24" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="P24" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q24" s="37"/>
+      <c r="R24" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="S24" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="T24" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="U24" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="V24" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="W24" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="X24" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y24" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z24" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA24" s="37"/>
+      <c r="AB24" s="37"/>
+      <c r="AC24" s="37"/>
+      <c r="AD24" s="37"/>
+      <c r="AE24" s="37"/>
+      <c r="AF24" s="37"/>
+      <c r="AG24" s="37"/>
+      <c r="AH24" s="37"/>
+      <c r="AI24" s="37"/>
+      <c r="AJ24" s="37"/>
+      <c r="AK24" s="37"/>
+      <c r="AL24" s="37"/>
+      <c r="AM24" s="37"/>
+      <c r="AN24" s="37"/>
+      <c r="AO24" s="37"/>
+      <c r="AP24" s="37"/>
+      <c r="AQ24" s="37"/>
+      <c r="AR24" s="37"/>
+      <c r="AS24" s="37"/>
+      <c r="AT24" s="37"/>
+      <c r="AU24" s="37"/>
+      <c r="AV24" s="37"/>
+      <c r="AW24" s="37"/>
+      <c r="AX24" s="37"/>
+      <c r="AY24" s="37"/>
+      <c r="AZ24" s="37"/>
+    </row>
+    <row r="25" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" t="s">
+        <v>30</v>
+      </c>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q25" s="21"/>
+      <c r="R25" s="21"/>
+      <c r="S25" s="21"/>
+      <c r="T25" s="21"/>
+      <c r="U25" s="21"/>
+      <c r="V25" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="W25" s="21"/>
+      <c r="X25" s="21"/>
+      <c r="Y25" s="21"/>
+      <c r="Z25" s="21"/>
+      <c r="AA25" s="21"/>
+      <c r="AB25" s="21"/>
+      <c r="AC25" s="21"/>
+      <c r="AD25" s="21"/>
+      <c r="AE25" s="21"/>
+      <c r="AF25" s="21"/>
+      <c r="AG25" s="21"/>
+      <c r="AH25" s="21"/>
+      <c r="AI25" s="21"/>
+      <c r="AJ25" s="21"/>
+      <c r="AK25" s="21"/>
+      <c r="AL25" s="21"/>
+      <c r="AM25" s="21"/>
+      <c r="AN25" s="21"/>
+      <c r="AO25" s="21"/>
+      <c r="AP25" s="21"/>
+    </row>
+    <row r="26" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="3"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="21"/>
+      <c r="P26" s="21"/>
+      <c r="Q26" s="21"/>
+      <c r="R26" s="21"/>
+      <c r="S26" s="21"/>
+      <c r="T26" s="21"/>
+      <c r="U26" s="21"/>
+      <c r="V26" s="21"/>
+      <c r="W26" s="21"/>
+      <c r="X26" s="21"/>
+      <c r="Y26" s="21"/>
+      <c r="Z26" s="21"/>
+      <c r="AA26" s="21"/>
+      <c r="AB26" s="21"/>
+      <c r="AC26" s="21"/>
+      <c r="AD26" s="21"/>
+      <c r="AE26" s="21"/>
+      <c r="AF26" s="21"/>
+      <c r="AG26" s="21"/>
+      <c r="AH26" s="21"/>
+      <c r="AI26" s="21"/>
+      <c r="AJ26" s="21"/>
+      <c r="AK26" s="21"/>
+      <c r="AL26" s="21"/>
+      <c r="AM26" s="21"/>
+      <c r="AN26" s="21"/>
+      <c r="AO26" s="21"/>
+      <c r="AP26" s="21"/>
+    </row>
+    <row r="27" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="29"/>
+      <c r="O27" s="29"/>
+      <c r="P27" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q27" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="R27" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="S27" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="T27" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="U27" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="V27" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="W27" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="X27" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y27" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z27" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA27" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB27" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC27" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD27" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE27" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF27" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG27" s="29"/>
+      <c r="AH27" s="29"/>
+      <c r="AI27" s="29"/>
+      <c r="AJ27" s="29"/>
+      <c r="AK27" s="29"/>
+      <c r="AL27" s="29"/>
+      <c r="AM27" s="29"/>
+      <c r="AN27" s="29"/>
+      <c r="AO27" s="29"/>
+      <c r="AP27" s="29"/>
+      <c r="AQ27" s="29"/>
+      <c r="AR27" s="29"/>
+      <c r="AS27" s="29"/>
+      <c r="AT27" s="29"/>
+      <c r="AU27" s="29"/>
+      <c r="AV27" s="29"/>
+      <c r="AW27" s="29"/>
+      <c r="AX27" s="29"/>
+      <c r="AY27" s="29"/>
+      <c r="AZ27" s="29"/>
+    </row>
+    <row r="28" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="P28" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q28" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="R28" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="S28" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="T28" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="U28" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="V28" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="W28" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="X28" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y28" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z28" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA28" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB28" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC28" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD28" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE28" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF28" s="21"/>
+      <c r="AG28" s="21"/>
+      <c r="AH28" s="21"/>
+      <c r="AI28" s="21"/>
+      <c r="AJ28" s="21"/>
+      <c r="AK28" s="21"/>
+      <c r="AL28" s="21"/>
+      <c r="AM28" s="21"/>
+      <c r="AN28" s="21"/>
+      <c r="AO28" s="21"/>
+      <c r="AP28" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>